<commit_message>
Fixed Class 1 Snag all others
</commit_message>
<xml_diff>
--- a/specifications/1_Fire/ScriptRules_Fire.xlsx
+++ b/specifications/1_Fire/ScriptRules_Fire.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="6" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -2417,20 +2417,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K952"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101.28515625" style="27" customWidth="1"/>
     <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="44.5703125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="25" customWidth="1"/>
-    <col min="5" max="5" width="41.42578125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="46.28515625" style="21" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" style="25" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="44.5703125" style="21" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="25" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="41.42578125" style="26" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" style="21" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" style="25" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="26" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="44.85546875" style="21" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="48" style="25" customWidth="1"/>
     <col min="11" max="11" width="36.5703125" style="26" customWidth="1"/>
@@ -11126,7 +11126,7 @@
         <v>3.125</v>
       </c>
       <c r="M34" s="13">
-        <f t="shared" ref="M34:M37" si="57">$E34*L34</f>
+        <f t="shared" ref="M34" si="57">$E34*L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="4">
@@ -11141,7 +11141,7 @@
         <v>1.875</v>
       </c>
       <c r="Q34" s="13">
-        <f t="shared" ref="Q34:Q37" si="60">$E34*P34</f>
+        <f t="shared" ref="Q34" si="60">$E34*P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="4">
@@ -11156,7 +11156,7 @@
         <v>3.125</v>
       </c>
       <c r="U34" s="13">
-        <f t="shared" ref="U34:U37" si="63">$E34*T34</f>
+        <f t="shared" ref="U34" si="63">$E34*T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="4">
@@ -11171,7 +11171,7 @@
         <v>3.75</v>
       </c>
       <c r="Y34" s="13">
-        <f t="shared" ref="Y34:Y37" si="66">$E34*X34</f>
+        <f t="shared" ref="Y34" si="66">$E34*X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="4">
@@ -11186,7 +11186,7 @@
         <v>3.125</v>
       </c>
       <c r="AC34" s="13">
-        <f t="shared" ref="AC34:AC37" si="69">$E34*AB34</f>
+        <f t="shared" ref="AC34" si="69">$E34*AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -11453,7 +11453,7 @@
         <v>1.25</v>
       </c>
       <c r="M37" s="13">
-        <f t="shared" ref="M37:M40" si="70">$E37*L37</f>
+        <f t="shared" ref="M37" si="70">$E37*L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="5">
@@ -11465,7 +11465,7 @@
         <v>0</v>
       </c>
       <c r="Q37" s="13">
-        <f t="shared" ref="Q37:Q40" si="71">$E37*P37</f>
+        <f t="shared" ref="Q37" si="71">$E37*P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="4">
@@ -11480,7 +11480,7 @@
         <v>0.625</v>
       </c>
       <c r="U37" s="13">
-        <f t="shared" ref="U37:U40" si="72">$E37*T37</f>
+        <f t="shared" ref="U37" si="72">$E37*T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="5">
@@ -11492,7 +11492,7 @@
         <v>0</v>
       </c>
       <c r="Y37" s="13">
-        <f t="shared" ref="Y37:Y40" si="73">$E37*X37</f>
+        <f t="shared" ref="Y37" si="73">$E37*X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="5">
@@ -11504,7 +11504,7 @@
         <v>0</v>
       </c>
       <c r="AC37" s="13">
-        <f t="shared" ref="AC37:AC40" si="74">$E37*AB37</f>
+        <f t="shared" ref="AC37" si="74">$E37*AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -13795,7 +13795,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="9">
-        <f t="shared" ref="M60:M80" si="101">L60</f>
+        <f t="shared" ref="M60:M77" si="101">L60</f>
         <v>0</v>
       </c>
       <c r="O60" s="5">
@@ -13807,7 +13807,7 @@
         <v>0</v>
       </c>
       <c r="Q60" s="9">
-        <f t="shared" ref="Q60:Q80" si="102">P60</f>
+        <f t="shared" ref="Q60:Q77" si="102">P60</f>
         <v>0</v>
       </c>
       <c r="R60" s="4">
@@ -13822,7 +13822,7 @@
         <v>2</v>
       </c>
       <c r="U60" s="9">
-        <f t="shared" ref="U60:U80" si="103">T60</f>
+        <f t="shared" ref="U60:U77" si="103">T60</f>
         <v>2</v>
       </c>
       <c r="W60" s="5">
@@ -13834,7 +13834,7 @@
         <v>0</v>
       </c>
       <c r="Y60" s="9">
-        <f t="shared" ref="Y60:Y80" si="104">X60</f>
+        <f t="shared" ref="Y60:Y77" si="104">X60</f>
         <v>0</v>
       </c>
       <c r="AA60" s="5">
@@ -13846,7 +13846,7 @@
         <v>0</v>
       </c>
       <c r="AC60" s="9">
-        <f t="shared" ref="AC60:AC80" si="105">AB60</f>
+        <f t="shared" ref="AC60:AC77" si="105">AB60</f>
         <v>0</v>
       </c>
     </row>
@@ -15642,11 +15642,11 @@
         <v>0.75</v>
       </c>
       <c r="L80" s="8">
-        <f t="shared" ref="L80:L93" si="132">$D80*K80</f>
+        <f t="shared" ref="L80:L81" si="132">$D80*K80</f>
         <v>1</v>
       </c>
       <c r="M80" s="9">
-        <f t="shared" ref="M80:M93" si="133">L80</f>
+        <f t="shared" ref="M80:M81" si="133">L80</f>
         <v>1</v>
       </c>
       <c r="N80" s="4">
@@ -15657,11 +15657,11 @@
         <v>1.875</v>
       </c>
       <c r="P80" s="8">
-        <f t="shared" ref="P80:P93" si="134">$D80*O80</f>
+        <f t="shared" ref="P80:P81" si="134">$D80*O80</f>
         <v>2.5</v>
       </c>
       <c r="Q80" s="9">
-        <f t="shared" ref="Q80:Q93" si="135">P80</f>
+        <f t="shared" ref="Q80:Q81" si="135">P80</f>
         <v>2.5</v>
       </c>
       <c r="R80" s="4">
@@ -15672,11 +15672,11 @@
         <v>0.75</v>
       </c>
       <c r="T80" s="8">
-        <f t="shared" ref="T80:T93" si="136">$D80*S80</f>
+        <f t="shared" ref="T80:T81" si="136">$D80*S80</f>
         <v>1</v>
       </c>
       <c r="U80" s="9">
-        <f t="shared" ref="U80:U93" si="137">T80</f>
+        <f t="shared" ref="U80:U81" si="137">T80</f>
         <v>1</v>
       </c>
       <c r="V80" s="4">
@@ -15687,11 +15687,11 @@
         <v>1.125</v>
       </c>
       <c r="X80" s="8">
-        <f t="shared" ref="X80:X93" si="138">$D80*W80</f>
+        <f t="shared" ref="X80:X81" si="138">$D80*W80</f>
         <v>1.5</v>
       </c>
       <c r="Y80" s="9">
-        <f t="shared" ref="Y80:Y93" si="139">X80</f>
+        <f t="shared" ref="Y80:Y81" si="139">X80</f>
         <v>1.5</v>
       </c>
       <c r="Z80" s="4">
@@ -15702,11 +15702,11 @@
         <v>1.5</v>
       </c>
       <c r="AB80" s="8">
-        <f t="shared" ref="AB80:AB93" si="140">$D80*AA80</f>
+        <f t="shared" ref="AB80:AB81" si="140">$D80*AA80</f>
         <v>2</v>
       </c>
       <c r="AC80" s="9">
-        <f t="shared" ref="AC80:AC93" si="141">AB80</f>
+        <f t="shared" ref="AC80:AC81" si="141">AB80</f>
         <v>2</v>
       </c>
     </row>
@@ -17226,7 +17226,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="8">
-        <f t="shared" ref="L3:L17" si="1">K3</f>
+        <f t="shared" ref="L3:L5" si="1">K3</f>
         <v>0</v>
       </c>
       <c r="M3" s="49">
@@ -17238,7 +17238,7 @@
         <v>0</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" ref="P3:P17" si="3">O3</f>
+        <f t="shared" ref="P3:P5" si="3">O3</f>
         <v>0</v>
       </c>
       <c r="Q3" s="49">
@@ -17253,7 +17253,7 @@
         <v>2.9</v>
       </c>
       <c r="T3" s="8">
-        <f t="shared" ref="T3:T17" si="5">S3</f>
+        <f t="shared" ref="T3:T5" si="5">S3</f>
         <v>2.9</v>
       </c>
       <c r="U3" s="49">
@@ -17268,7 +17268,7 @@
         <v>14</v>
       </c>
       <c r="X3" s="8">
-        <f t="shared" ref="X3:X17" si="7">W3</f>
+        <f t="shared" ref="X3:X5" si="7">W3</f>
         <v>14</v>
       </c>
       <c r="Y3" s="49">
@@ -17283,7 +17283,7 @@
         <v>12</v>
       </c>
       <c r="AB3" s="8">
-        <f t="shared" ref="AB3:AB17" si="9">AA3</f>
+        <f t="shared" ref="AB3:AB5" si="9">AA3</f>
         <v>12</v>
       </c>
       <c r="AC3" s="49">
@@ -17713,7 +17713,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" ref="L8:L22" si="11">K8</f>
+        <f t="shared" ref="L8:L10" si="11">K8</f>
         <v>0</v>
       </c>
       <c r="M8" s="49">
@@ -17725,7 +17725,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" ref="P8:P22" si="12">O8</f>
+        <f t="shared" ref="P8:P10" si="12">O8</f>
         <v>0</v>
       </c>
       <c r="Q8" s="49">
@@ -17737,7 +17737,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" ref="T8:T22" si="13">S8</f>
+        <f t="shared" ref="T8:T10" si="13">S8</f>
         <v>0</v>
       </c>
       <c r="U8" s="49">
@@ -17752,7 +17752,7 @@
         <v>7.5</v>
       </c>
       <c r="X8" s="8">
-        <f t="shared" ref="X8:X22" si="14">W8</f>
+        <f t="shared" ref="X8:X10" si="14">W8</f>
         <v>7.5</v>
       </c>
       <c r="Y8" s="49">
@@ -17764,7 +17764,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="8">
-        <f t="shared" ref="AB8:AB22" si="15">AA8</f>
+        <f t="shared" ref="AB8:AB10" si="15">AA8</f>
         <v>0</v>
       </c>
       <c r="AC8" s="49">
@@ -18158,7 +18158,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" ref="L13:L27" si="16">K13</f>
+        <f t="shared" ref="L13:L15" si="16">K13</f>
         <v>0</v>
       </c>
       <c r="M13" s="49">
@@ -18170,7 +18170,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" ref="P13:P27" si="17">O13</f>
+        <f t="shared" ref="P13:P15" si="17">O13</f>
         <v>0</v>
       </c>
       <c r="Q13" s="49">
@@ -18185,7 +18185,7 @@
         <v>0.5</v>
       </c>
       <c r="T13" s="8">
-        <f t="shared" ref="T13:T27" si="18">S13</f>
+        <f t="shared" ref="T13:T15" si="18">S13</f>
         <v>0.5</v>
       </c>
       <c r="U13" s="49">
@@ -18200,7 +18200,7 @@
         <v>1.7</v>
       </c>
       <c r="X13" s="8">
-        <f t="shared" ref="X13:X27" si="19">W13</f>
+        <f t="shared" ref="X13:X15" si="19">W13</f>
         <v>1.7</v>
       </c>
       <c r="Y13" s="49">
@@ -18215,7 +18215,7 @@
         <v>1</v>
       </c>
       <c r="AB13" s="8">
-        <f t="shared" ref="AB13:AB27" si="20">AA13</f>
+        <f t="shared" ref="AB13:AB15" si="20">AA13</f>
         <v>1</v>
       </c>
       <c r="AC13" s="49">
@@ -19485,7 +19485,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="49">
-        <f t="shared" ref="M27:M29" si="45">L19</f>
+        <f t="shared" ref="M27" si="45">L19</f>
         <v>0</v>
       </c>
       <c r="O27" s="5">
@@ -19497,7 +19497,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="49">
-        <f t="shared" ref="Q27:Q29" si="46">P19</f>
+        <f t="shared" ref="Q27" si="46">P19</f>
         <v>0</v>
       </c>
       <c r="R27" s="4">
@@ -19512,7 +19512,7 @@
         <v>25</v>
       </c>
       <c r="U27" s="49">
-        <f t="shared" ref="U27:U29" si="47">T19</f>
+        <f t="shared" ref="U27" si="47">T19</f>
         <v>25</v>
       </c>
       <c r="V27" s="4">
@@ -19527,7 +19527,7 @@
         <v>55</v>
       </c>
       <c r="Y27" s="49">
-        <f t="shared" ref="Y27:Y29" si="48">X19</f>
+        <f t="shared" ref="Y27" si="48">X19</f>
         <v>50</v>
       </c>
       <c r="Z27" s="4">
@@ -19542,7 +19542,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="49">
-        <f t="shared" ref="AC27:AC29" si="49">AB19</f>
+        <f t="shared" ref="AC27" si="49">AB19</f>
         <v>78</v>
       </c>
     </row>
@@ -19971,7 +19971,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="8">
-        <f t="shared" ref="L32:L39" si="61">K32</f>
+        <f t="shared" ref="L32:L33" si="61">K32</f>
         <v>0</v>
       </c>
       <c r="M32" s="49">
@@ -19983,7 +19983,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="8">
-        <f t="shared" ref="P32:P39" si="62">O32</f>
+        <f t="shared" ref="P32:P33" si="62">O32</f>
         <v>0</v>
       </c>
       <c r="Q32" s="49">
@@ -19998,7 +19998,7 @@
         <v>4</v>
       </c>
       <c r="T32" s="8">
-        <f t="shared" ref="T32:T39" si="63">S32</f>
+        <f t="shared" ref="T32:T33" si="63">S32</f>
         <v>4</v>
       </c>
       <c r="U32" s="49">
@@ -20013,7 +20013,7 @@
         <v>15</v>
       </c>
       <c r="X32" s="8">
-        <f t="shared" ref="X32:X39" si="64">W32</f>
+        <f t="shared" ref="X32:X33" si="64">W32</f>
         <v>15</v>
       </c>
       <c r="Y32" s="49">
@@ -20025,7 +20025,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="8">
-        <f t="shared" ref="AB32:AB39" si="65">AA32</f>
+        <f t="shared" ref="AB32:AB33" si="65">AA32</f>
         <v>0</v>
       </c>
       <c r="AC32" s="49">
@@ -20160,75 +20160,75 @@
         <v>5</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" ref="K34:K58" si="70">$C34*J34</f>
+        <f t="shared" ref="K34:K39" si="70">$C34*J34</f>
         <v>1.25</v>
       </c>
       <c r="L34" s="8">
-        <f t="shared" ref="L34:L37" si="71">$D34*K34</f>
+        <f t="shared" ref="L34" si="71">$D34*K34</f>
         <v>1.875</v>
       </c>
       <c r="M34" s="50">
-        <f t="shared" ref="M34:M55" si="72">$E34*L34</f>
+        <f t="shared" ref="M34" si="72">$E34*L34</f>
         <v>5</v>
       </c>
       <c r="N34" s="4">
         <v>3</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" ref="O34:O58" si="73">$C34*N34</f>
+        <f t="shared" ref="O34:O39" si="73">$C34*N34</f>
         <v>0.75</v>
       </c>
       <c r="P34" s="8">
-        <f t="shared" ref="P34:P37" si="74">$D34*O34</f>
+        <f t="shared" ref="P34" si="74">$D34*O34</f>
         <v>1.125</v>
       </c>
       <c r="Q34" s="50">
-        <f t="shared" ref="Q34:Q55" si="75">$E34*P34</f>
+        <f t="shared" ref="Q34" si="75">$E34*P34</f>
         <v>3</v>
       </c>
       <c r="R34" s="4">
         <v>5</v>
       </c>
       <c r="S34" s="5">
-        <f t="shared" ref="S34:S58" si="76">$C34*R34</f>
+        <f t="shared" ref="S34:S39" si="76">$C34*R34</f>
         <v>1.25</v>
       </c>
       <c r="T34" s="8">
-        <f t="shared" ref="T34:T37" si="77">$D34*S34</f>
+        <f t="shared" ref="T34" si="77">$D34*S34</f>
         <v>1.875</v>
       </c>
       <c r="U34" s="50">
-        <f t="shared" ref="U34:U55" si="78">$E34*T34</f>
+        <f t="shared" ref="U34" si="78">$E34*T34</f>
         <v>5</v>
       </c>
       <c r="V34" s="4">
         <v>6</v>
       </c>
       <c r="W34" s="5">
-        <f t="shared" ref="W34:W58" si="79">$C34*V34</f>
+        <f t="shared" ref="W34:W39" si="79">$C34*V34</f>
         <v>1.5</v>
       </c>
       <c r="X34" s="8">
-        <f t="shared" ref="X34:X37" si="80">$D34*W34</f>
+        <f t="shared" ref="X34" si="80">$D34*W34</f>
         <v>2.25</v>
       </c>
       <c r="Y34" s="50">
-        <f t="shared" ref="Y34:Y55" si="81">$E34*X34</f>
+        <f t="shared" ref="Y34" si="81">$E34*X34</f>
         <v>6</v>
       </c>
       <c r="Z34" s="4">
         <v>5</v>
       </c>
       <c r="AA34" s="5">
-        <f t="shared" ref="AA34:AA58" si="82">$C34*Z34</f>
+        <f t="shared" ref="AA34:AA39" si="82">$C34*Z34</f>
         <v>1.25</v>
       </c>
       <c r="AB34" s="8">
-        <f t="shared" ref="AB34:AB37" si="83">$D34*AA34</f>
+        <f t="shared" ref="AB34" si="83">$D34*AA34</f>
         <v>1.875</v>
       </c>
       <c r="AC34" s="50">
-        <f t="shared" ref="AC34:AC55" si="84">$E34*AB34</f>
+        <f t="shared" ref="AC34" si="84">$E34*AB34</f>
         <v>5</v>
       </c>
     </row>
@@ -20491,11 +20491,11 @@
         <v>0.5</v>
       </c>
       <c r="L37" s="8">
-        <f t="shared" ref="L37:L40" si="85">$D37*K37</f>
+        <f t="shared" ref="L37" si="85">$D37*K37</f>
         <v>0.75</v>
       </c>
       <c r="M37" s="50">
-        <f t="shared" ref="M37:M58" si="86">$E37*L37</f>
+        <f t="shared" ref="M37" si="86">$E37*L37</f>
         <v>2</v>
       </c>
       <c r="O37" s="5">
@@ -20503,11 +20503,11 @@
         <v>0</v>
       </c>
       <c r="P37" s="8">
-        <f t="shared" ref="P37:P40" si="87">$D37*O37</f>
+        <f t="shared" ref="P37" si="87">$D37*O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="50">
-        <f t="shared" ref="Q37:Q58" si="88">$E37*P37</f>
+        <f t="shared" ref="Q37" si="88">$E37*P37</f>
         <v>0</v>
       </c>
       <c r="R37" s="4">
@@ -20518,11 +20518,11 @@
         <v>0.25</v>
       </c>
       <c r="T37" s="8">
-        <f t="shared" ref="T37:T40" si="89">$D37*S37</f>
+        <f t="shared" ref="T37" si="89">$D37*S37</f>
         <v>0.375</v>
       </c>
       <c r="U37" s="50">
-        <f t="shared" ref="U37:U58" si="90">$E37*T37</f>
+        <f t="shared" ref="U37" si="90">$E37*T37</f>
         <v>1</v>
       </c>
       <c r="W37" s="5">
@@ -20530,11 +20530,11 @@
         <v>0</v>
       </c>
       <c r="X37" s="8">
-        <f t="shared" ref="X37:X40" si="91">$D37*W37</f>
+        <f t="shared" ref="X37" si="91">$D37*W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="50">
-        <f t="shared" ref="Y37:Y58" si="92">$E37*X37</f>
+        <f t="shared" ref="Y37" si="92">$E37*X37</f>
         <v>0</v>
       </c>
       <c r="AA37" s="5">
@@ -20542,11 +20542,11 @@
         <v>0</v>
       </c>
       <c r="AB37" s="8">
-        <f t="shared" ref="AB37:AB40" si="93">$D37*AA37</f>
+        <f t="shared" ref="AB37" si="93">$D37*AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="50">
-        <f t="shared" ref="AC37:AC58" si="94">$E37*AB37</f>
+        <f t="shared" ref="AC37" si="94">$E37*AB37</f>
         <v>0</v>
       </c>
     </row>
@@ -20890,75 +20890,75 @@
         <v>0.125</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" ref="K41:K65" si="97">$C41*J41</f>
+        <f t="shared" ref="K41:K47" si="97">$C41*J41</f>
         <v>0</v>
       </c>
       <c r="L41" s="8">
-        <f t="shared" ref="L41:L46" si="98">$D41*K41</f>
+        <f t="shared" ref="L41:L42" si="98">$D41*K41</f>
         <v>0</v>
       </c>
       <c r="M41" s="50">
-        <f t="shared" ref="M41:M62" si="99">$E41*L41</f>
+        <f t="shared" ref="M41" si="99">$E41*L41</f>
         <v>0</v>
       </c>
       <c r="N41" s="4">
         <v>1</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" ref="O41:O65" si="100">$C41*N41</f>
+        <f t="shared" ref="O41:O47" si="100">$C41*N41</f>
         <v>0.25</v>
       </c>
       <c r="P41" s="8">
-        <f t="shared" ref="P41:P46" si="101">$D41*O41</f>
+        <f t="shared" ref="P41:P42" si="101">$D41*O41</f>
         <v>1</v>
       </c>
       <c r="Q41" s="50">
-        <f t="shared" ref="Q41:Q62" si="102">$E41*P41</f>
+        <f t="shared" ref="Q41" si="102">$E41*P41</f>
         <v>1.25</v>
       </c>
       <c r="R41" s="4">
         <v>0.01</v>
       </c>
       <c r="S41" s="5">
-        <f t="shared" ref="S41:S65" si="103">$C41*R41</f>
+        <f t="shared" ref="S41:S47" si="103">$C41*R41</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="T41" s="8">
-        <f t="shared" ref="T41:T46" si="104">$D41*S41</f>
+        <f t="shared" ref="T41:T42" si="104">$D41*S41</f>
         <v>0.01</v>
       </c>
       <c r="U41" s="50">
-        <f t="shared" ref="U41:U62" si="105">$E41*T41</f>
+        <f t="shared" ref="U41" si="105">$E41*T41</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="V41" s="4">
         <v>0.4</v>
       </c>
       <c r="W41" s="5">
-        <f t="shared" ref="W41:W65" si="106">$C41*V41</f>
+        <f t="shared" ref="W41:W47" si="106">$C41*V41</f>
         <v>0.1</v>
       </c>
       <c r="X41" s="8">
-        <f t="shared" ref="X41:X46" si="107">$D41*W41</f>
+        <f t="shared" ref="X41:X42" si="107">$D41*W41</f>
         <v>0.4</v>
       </c>
       <c r="Y41" s="50">
-        <f t="shared" ref="Y41:Y62" si="108">$E41*X41</f>
+        <f t="shared" ref="Y41" si="108">$E41*X41</f>
         <v>0.5</v>
       </c>
       <c r="Z41" s="4">
         <v>0.1</v>
       </c>
       <c r="AA41" s="5">
-        <f t="shared" ref="AA41:AA65" si="109">$C41*Z41</f>
+        <f t="shared" ref="AA41:AA47" si="109">$C41*Z41</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="AB41" s="8">
-        <f t="shared" ref="AB41:AB46" si="110">$D41*AA41</f>
+        <f t="shared" ref="AB41:AB42" si="110">$D41*AA41</f>
         <v>0.1</v>
       </c>
       <c r="AC41" s="50">
-        <f t="shared" ref="AC41:AC62" si="111">$E41*AB41</f>
+        <f t="shared" ref="AC41" si="111">$E41*AB41</f>
         <v>0.125</v>
       </c>
     </row>
@@ -21212,7 +21212,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="8">
-        <f t="shared" ref="L44:L49" si="112">$D44*K44</f>
+        <f t="shared" ref="L44:L46" si="112">$D44*K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="50">
@@ -21227,7 +21227,7 @@
         <v>0.25</v>
       </c>
       <c r="P44" s="8">
-        <f t="shared" ref="P44:P49" si="113">$D44*O44</f>
+        <f t="shared" ref="P44:P46" si="113">$D44*O44</f>
         <v>1</v>
       </c>
       <c r="Q44" s="50">
@@ -21242,7 +21242,7 @@
         <v>0.125</v>
       </c>
       <c r="T44" s="8">
-        <f t="shared" ref="T44:T49" si="114">$D44*S44</f>
+        <f t="shared" ref="T44:T46" si="114">$D44*S44</f>
         <v>0.5</v>
       </c>
       <c r="U44" s="50">
@@ -21254,7 +21254,7 @@
         <v>0</v>
       </c>
       <c r="X44" s="8">
-        <f t="shared" ref="X44:X49" si="115">$D44*W44</f>
+        <f t="shared" ref="X44:X46" si="115">$D44*W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="50">
@@ -21269,7 +21269,7 @@
         <v>0.25</v>
       </c>
       <c r="AB44" s="8">
-        <f t="shared" ref="AB44:AB49" si="116">$D44*AA44</f>
+        <f t="shared" ref="AB44:AB46" si="116">$D44*AA44</f>
         <v>1</v>
       </c>
       <c r="AC44" s="50">
@@ -21319,7 +21319,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="50">
-        <f t="shared" ref="M45:M66" si="117">$E45*L45</f>
+        <f t="shared" ref="M45" si="117">$E45*L45</f>
         <v>0</v>
       </c>
       <c r="N45" s="4">
@@ -21334,7 +21334,7 @@
         <v>0.01</v>
       </c>
       <c r="Q45" s="50">
-        <f t="shared" ref="Q45:Q66" si="118">$E45*P45</f>
+        <f t="shared" ref="Q45" si="118">$E45*P45</f>
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="R45" s="4">
@@ -21349,7 +21349,7 @@
         <v>0.02</v>
       </c>
       <c r="U45" s="50">
-        <f t="shared" ref="U45:U66" si="119">$E45*T45</f>
+        <f t="shared" ref="U45" si="119">$E45*T45</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="W45" s="5">
@@ -21361,7 +21361,7 @@
         <v>0</v>
       </c>
       <c r="Y45" s="50">
-        <f t="shared" ref="Y45:Y66" si="120">$E45*X45</f>
+        <f t="shared" ref="Y45" si="120">$E45*X45</f>
         <v>0</v>
       </c>
       <c r="Z45" s="4">
@@ -21376,7 +21376,7 @@
         <v>0.1</v>
       </c>
       <c r="AC45" s="50">
-        <f t="shared" ref="AC45:AC66" si="121">$E45*AB45</f>
+        <f t="shared" ref="AC45" si="121">$E45*AB45</f>
         <v>0.125</v>
       </c>
     </row>
@@ -21631,7 +21631,7 @@
         <v>0.3125</v>
       </c>
       <c r="M48" s="50">
-        <f t="shared" ref="M48:M69" si="124">$E48*L48</f>
+        <f t="shared" ref="M48:M55" si="124">$E48*L48</f>
         <v>1</v>
       </c>
       <c r="O48" s="5">
@@ -21643,7 +21643,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="50">
-        <f t="shared" ref="Q48:Q69" si="126">$E48*P48</f>
+        <f t="shared" ref="Q48:Q55" si="126">$E48*P48</f>
         <v>0</v>
       </c>
       <c r="R48" s="4">
@@ -21658,7 +21658,7 @@
         <v>0.15625</v>
       </c>
       <c r="U48" s="50">
-        <f t="shared" ref="U48:U69" si="128">$E48*T48</f>
+        <f t="shared" ref="U48:U55" si="128">$E48*T48</f>
         <v>0.5</v>
       </c>
       <c r="V48" s="4">
@@ -21673,7 +21673,7 @@
         <v>0.3125</v>
       </c>
       <c r="Y48" s="50">
-        <f t="shared" ref="Y48:Y69" si="130">$E48*X48</f>
+        <f t="shared" ref="Y48:Y55" si="130">$E48*X48</f>
         <v>1</v>
       </c>
       <c r="Z48" s="4">
@@ -21688,7 +21688,7 @@
         <v>0.15625</v>
       </c>
       <c r="AC48" s="50">
-        <f t="shared" ref="AC48:AC69" si="132">$E48*AB48</f>
+        <f t="shared" ref="AC48:AC55" si="132">$E48*AB48</f>
         <v>0.5</v>
       </c>
     </row>
@@ -21729,7 +21729,7 @@
         <v>50</v>
       </c>
       <c r="K49" s="5">
-        <f t="shared" ref="K49:K73" si="133">$C49*J49</f>
+        <f t="shared" ref="K49:K58" si="133">$C49*J49</f>
         <v>12.5</v>
       </c>
       <c r="L49" s="8">
@@ -21741,7 +21741,7 @@
         <v>50</v>
       </c>
       <c r="O49" s="5">
-        <f t="shared" ref="O49:O73" si="134">$C49*N49</f>
+        <f t="shared" ref="O49:O58" si="134">$C49*N49</f>
         <v>0</v>
       </c>
       <c r="P49" s="8">
@@ -21756,7 +21756,7 @@
         <v>30</v>
       </c>
       <c r="S49" s="5">
-        <f t="shared" ref="S49:S73" si="135">$C49*R49</f>
+        <f t="shared" ref="S49:S58" si="135">$C49*R49</f>
         <v>7.5</v>
       </c>
       <c r="T49" s="8">
@@ -21771,7 +21771,7 @@
         <v>40</v>
       </c>
       <c r="W49" s="5">
-        <f t="shared" ref="W49:W73" si="136">$C49*V49</f>
+        <f t="shared" ref="W49:W58" si="136">$C49*V49</f>
         <v>10</v>
       </c>
       <c r="X49" s="8">
@@ -21786,7 +21786,7 @@
         <v>15</v>
       </c>
       <c r="AA49" s="5">
-        <f t="shared" ref="AA49:AA73" si="137">$C49*Z49</f>
+        <f t="shared" ref="AA49:AA58" si="137">$C49*Z49</f>
         <v>3.75</v>
       </c>
       <c r="AB49" s="8">
@@ -22853,7 +22853,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="49">
-        <f t="shared" ref="M60:M78" si="144">L60</f>
+        <f t="shared" ref="M60:M77" si="144">L60</f>
         <v>0</v>
       </c>
       <c r="O60" s="5">
@@ -22865,7 +22865,7 @@
         <v>0</v>
       </c>
       <c r="Q60" s="49">
-        <f t="shared" ref="Q60:Q78" si="145">P60</f>
+        <f t="shared" ref="Q60:Q77" si="145">P60</f>
         <v>0</v>
       </c>
       <c r="R60" s="4">
@@ -22880,7 +22880,7 @@
         <v>2</v>
       </c>
       <c r="U60" s="49">
-        <f t="shared" ref="U60:U78" si="146">T60</f>
+        <f t="shared" ref="U60:U77" si="146">T60</f>
         <v>2</v>
       </c>
       <c r="W60" s="5">
@@ -22892,7 +22892,7 @@
         <v>0</v>
       </c>
       <c r="Y60" s="49">
-        <f t="shared" ref="Y60:Y78" si="147">X60</f>
+        <f t="shared" ref="Y60:Y77" si="147">X60</f>
         <v>0</v>
       </c>
       <c r="AA60" s="5">
@@ -22904,7 +22904,7 @@
         <v>0</v>
       </c>
       <c r="AC60" s="49">
-        <f t="shared" ref="AC60:AC78" si="148">AB60</f>
+        <f t="shared" ref="AC60:AC77" si="148">AB60</f>
         <v>0</v>
       </c>
     </row>
@@ -26003,7 +26003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="AD2" sqref="AD2"/>
     </sheetView>
   </sheetViews>
@@ -27663,8 +27663,8 @@
         <v>9.6</v>
       </c>
       <c r="I18" s="42">
-        <f>H22</f>
-        <v>9.6</v>
+        <f>$E18*H18</f>
+        <v>0</v>
       </c>
       <c r="K18" s="5">
         <f>J18</f>
@@ -27675,7 +27675,7 @@
         <v>0</v>
       </c>
       <c r="M18" s="42">
-        <f>L22</f>
+        <f>$E18*L18</f>
         <v>0</v>
       </c>
       <c r="O18" s="5">
@@ -27687,7 +27687,7 @@
         <v>0</v>
       </c>
       <c r="Q18" s="42">
-        <f>P22</f>
+        <f>$E18*P18</f>
         <v>0</v>
       </c>
       <c r="R18" s="4">
@@ -27702,8 +27702,8 @@
         <v>2.9</v>
       </c>
       <c r="U18" s="42">
-        <f>T22</f>
-        <v>2.9</v>
+        <f>$E18*T18</f>
+        <v>0</v>
       </c>
       <c r="V18" s="4">
         <v>13</v>
@@ -27717,8 +27717,8 @@
         <v>9</v>
       </c>
       <c r="Y18" s="42">
-        <f>X22</f>
-        <v>9</v>
+        <f>$E18*X18</f>
+        <v>0</v>
       </c>
       <c r="AA18" s="5">
         <f>Z18</f>
@@ -27729,8 +27729,8 @@
         <v>12</v>
       </c>
       <c r="AC18" s="42">
-        <f>AB22</f>
-        <v>12</v>
+        <f>$E18*AB18</f>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -27757,8 +27757,8 @@
         <v>100</v>
       </c>
       <c r="I19" s="42">
-        <f>H23</f>
-        <v>100</v>
+        <f>$E19*H19</f>
+        <v>0</v>
       </c>
       <c r="K19" s="5">
         <f>J19</f>
@@ -27769,7 +27769,7 @@
         <v>0</v>
       </c>
       <c r="M19" s="42">
-        <f>L23</f>
+        <f>$E19*L19</f>
         <v>0</v>
       </c>
       <c r="O19" s="5">
@@ -27781,7 +27781,7 @@
         <v>0</v>
       </c>
       <c r="Q19" s="42">
-        <f>P23</f>
+        <f>$E19*P19</f>
         <v>0</v>
       </c>
       <c r="R19" s="4">
@@ -27796,8 +27796,8 @@
         <v>25</v>
       </c>
       <c r="U19" s="42">
-        <f>T23</f>
-        <v>25</v>
+        <f>$E19*T19</f>
+        <v>0</v>
       </c>
       <c r="V19" s="4">
         <v>55</v>
@@ -27811,8 +27811,8 @@
         <v>50</v>
       </c>
       <c r="Y19" s="42">
-        <f>X23</f>
-        <v>50</v>
+        <f>$E19*X19</f>
+        <v>0</v>
       </c>
       <c r="AA19" s="5">
         <f>Z19</f>
@@ -27823,8 +27823,8 @@
         <v>78</v>
       </c>
       <c r="AC19" s="42">
-        <f>AB23</f>
-        <v>78</v>
+        <f>$E19*AB19</f>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -27851,8 +27851,8 @@
         <v>9</v>
       </c>
       <c r="I20" s="42">
-        <f>H25</f>
-        <v>9.3000000000000007</v>
+        <f>$E20*H20</f>
+        <v>0</v>
       </c>
       <c r="K20" s="5">
         <f>J20</f>
@@ -27863,7 +27863,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="42">
-        <f>L25</f>
+        <f>$E20*L20</f>
         <v>0</v>
       </c>
       <c r="O20" s="5">
@@ -27875,7 +27875,7 @@
         <v>0</v>
       </c>
       <c r="Q20" s="42">
-        <f>P25</f>
+        <f>$E20*P20</f>
         <v>0</v>
       </c>
       <c r="R20" s="4">
@@ -27890,8 +27890,8 @@
         <v>2625</v>
       </c>
       <c r="U20" s="42">
-        <f>T25</f>
-        <v>2712.5</v>
+        <f>$E20*T20</f>
+        <v>0</v>
       </c>
       <c r="V20" s="4">
         <v>5</v>
@@ -27905,8 +27905,8 @@
         <v>151.25</v>
       </c>
       <c r="Y20" s="42">
-        <f>X25</f>
-        <v>156.125</v>
+        <f>$E20*X20</f>
+        <v>0</v>
       </c>
       <c r="AA20" s="5">
         <f>Z20</f>
@@ -27917,8 +27917,8 @@
         <v>75</v>
       </c>
       <c r="AC20" s="42">
-        <f>AB25</f>
-        <v>77.5</v>
+        <f>$E20*AB20</f>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -39235,7 +39235,7 @@
       </c>
       <c r="K18">
         <f>'13_Fire_HighSeverity'!I18</f>
-        <v>9.6</v>
+        <v>0</v>
       </c>
       <c r="L18">
         <f>'11_Fire_LowSeverity'!J18</f>
@@ -39355,7 +39355,7 @@
       </c>
       <c r="AO18">
         <f>'13_Fire_HighSeverity'!U18</f>
-        <v>2.9</v>
+        <v>0</v>
       </c>
       <c r="AP18">
         <f>'11_Fire_LowSeverity'!V18</f>
@@ -39395,7 +39395,7 @@
       </c>
       <c r="AY18">
         <f>'13_Fire_HighSeverity'!Y18</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AZ18">
         <f>'11_Fire_LowSeverity'!Z18</f>
@@ -39435,7 +39435,7 @@
       </c>
       <c r="BI18">
         <f>'13_Fire_HighSeverity'!AC18</f>
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:61" x14ac:dyDescent="0.25">
@@ -39481,7 +39481,7 @@
       </c>
       <c r="K19">
         <f>'13_Fire_HighSeverity'!I19</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="L19">
         <f>'11_Fire_LowSeverity'!J19</f>
@@ -39601,7 +39601,7 @@
       </c>
       <c r="AO19">
         <f>'13_Fire_HighSeverity'!U19</f>
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="AP19">
         <f>'11_Fire_LowSeverity'!V19</f>
@@ -39641,7 +39641,7 @@
       </c>
       <c r="AY19">
         <f>'13_Fire_HighSeverity'!Y19</f>
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AZ19">
         <f>'11_Fire_LowSeverity'!Z19</f>
@@ -39681,7 +39681,7 @@
       </c>
       <c r="BI19">
         <f>'13_Fire_HighSeverity'!AC19</f>
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:61" x14ac:dyDescent="0.25">
@@ -39727,7 +39727,7 @@
       </c>
       <c r="K20">
         <f>'13_Fire_HighSeverity'!I20</f>
-        <v>9.3000000000000007</v>
+        <v>0</v>
       </c>
       <c r="L20">
         <f>'11_Fire_LowSeverity'!J20</f>
@@ -39847,7 +39847,7 @@
       </c>
       <c r="AO20">
         <f>'13_Fire_HighSeverity'!U20</f>
-        <v>2712.5</v>
+        <v>0</v>
       </c>
       <c r="AP20">
         <f>'11_Fire_LowSeverity'!V20</f>
@@ -39887,7 +39887,7 @@
       </c>
       <c r="AY20">
         <f>'13_Fire_HighSeverity'!Y20</f>
-        <v>156.125</v>
+        <v>0</v>
       </c>
       <c r="AZ20">
         <f>'11_Fire_LowSeverity'!Z20</f>
@@ -39927,7 +39927,7 @@
       </c>
       <c r="BI20">
         <f>'13_Fire_HighSeverity'!AC20</f>
-        <v>77.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:61" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Corrected fire low severity Class 1 Snags with Foliage density equation
</commit_message>
<xml_diff>
--- a/specifications/1_Fire/ScriptRules_Fire.xlsx
+++ b/specifications/1_Fire/ScriptRules_Fire.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -7953,8 +7953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9836,7 +9836,7 @@
       </c>
       <c r="X20" s="8">
         <f>W25</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="Y20" s="9">
         <f>$E20*X20</f>
@@ -10235,7 +10235,7 @@
       </c>
       <c r="E25" s="36"/>
       <c r="G25" s="5">
-        <f>(0.1*F7)+(0.1*F12)</f>
+        <f>F25+(0.1*F7)+(0.1*F12)</f>
         <v>1.2000000000000002</v>
       </c>
       <c r="H25" s="8">
@@ -10247,7 +10247,7 @@
         <v>0</v>
       </c>
       <c r="K25" s="5">
-        <f>(0.1*J7)+(0.1*J12)</f>
+        <f>J25+(0.1*J7)+(0.1*J12)</f>
         <v>0</v>
       </c>
       <c r="L25" s="8">
@@ -10259,7 +10259,7 @@
         <v>0</v>
       </c>
       <c r="O25" s="5">
-        <f>(0.1*N7)+(0.1*N12)</f>
+        <f>N25+(0.1*N7)+(0.1*N12)</f>
         <v>0</v>
       </c>
       <c r="P25" s="8">
@@ -10271,7 +10271,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="5">
-        <f>(0.1*R7)+(0.1*R12)</f>
+        <f>R25+(0.1*R7)+(0.1*R12)</f>
         <v>350</v>
       </c>
       <c r="T25" s="8">
@@ -10286,8 +10286,8 @@
         <v>5</v>
       </c>
       <c r="W25" s="5">
-        <f>(0.1*V7)+(0.1*V12)</f>
-        <v>19.5</v>
+        <f>V25+(0.1*V7)+(0.1*V12)</f>
+        <v>24.5</v>
       </c>
       <c r="X25" s="8">
         <f>$D25*W25</f>
@@ -10298,7 +10298,7 @@
         <v>0</v>
       </c>
       <c r="AA25" s="5">
-        <f>(0.1*Z7)+(0.1*Z12)</f>
+        <f>Z25+(0.1*Z7)+(0.1*Z12)</f>
         <v>10</v>
       </c>
       <c r="AB25" s="8">
@@ -10583,7 +10583,7 @@
       </c>
       <c r="Y28" s="9">
         <f t="shared" si="30"/>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="Z28" s="4">
         <v>3</v>
@@ -16969,8 +16969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26003,8 +26003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26260,7 +26260,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="8">
-        <f t="shared" ref="L3:L17" si="1">K3</f>
+        <f t="shared" ref="L3:L5" si="1">K3</f>
         <v>0</v>
       </c>
       <c r="M3" s="9">
@@ -26272,7 +26272,7 @@
         <v>0</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" ref="P3:P17" si="3">O3</f>
+        <f t="shared" ref="P3:P5" si="3">O3</f>
         <v>0</v>
       </c>
       <c r="Q3" s="9">
@@ -26287,7 +26287,7 @@
         <v>2.9</v>
       </c>
       <c r="T3" s="8">
-        <f t="shared" ref="T3:T17" si="5">S3</f>
+        <f t="shared" ref="T3:T5" si="5">S3</f>
         <v>2.9</v>
       </c>
       <c r="U3" s="9">
@@ -26302,7 +26302,7 @@
         <v>14</v>
       </c>
       <c r="X3" s="8">
-        <f t="shared" ref="X3:X17" si="7">W3</f>
+        <f t="shared" ref="X3:X5" si="7">W3</f>
         <v>14</v>
       </c>
       <c r="Y3" s="9">
@@ -26317,7 +26317,7 @@
         <v>12</v>
       </c>
       <c r="AB3" s="8">
-        <f t="shared" ref="AB3:AB17" si="9">AA3</f>
+        <f t="shared" ref="AB3:AB5" si="9">AA3</f>
         <v>12</v>
       </c>
       <c r="AC3" s="9">
@@ -26747,7 +26747,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" ref="L8:L22" si="11">K8</f>
+        <f t="shared" ref="L8:L10" si="11">K8</f>
         <v>0</v>
       </c>
       <c r="M8" s="9">
@@ -26759,7 +26759,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" ref="P8:P22" si="12">O8</f>
+        <f t="shared" ref="P8:P10" si="12">O8</f>
         <v>0</v>
       </c>
       <c r="Q8" s="9">
@@ -26771,7 +26771,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" ref="T8:T22" si="13">S8</f>
+        <f t="shared" ref="T8:T10" si="13">S8</f>
         <v>0</v>
       </c>
       <c r="U8" s="9">
@@ -26786,7 +26786,7 @@
         <v>7.5</v>
       </c>
       <c r="X8" s="8">
-        <f t="shared" ref="X8:X22" si="14">W8</f>
+        <f t="shared" ref="X8:X10" si="14">W8</f>
         <v>7.5</v>
       </c>
       <c r="Y8" s="9">
@@ -26798,7 +26798,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="8">
-        <f t="shared" ref="AB8:AB22" si="15">AA8</f>
+        <f t="shared" ref="AB8:AB10" si="15">AA8</f>
         <v>0</v>
       </c>
       <c r="AC8" s="9">
@@ -27192,7 +27192,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" ref="L13:L27" si="16">K13</f>
+        <f t="shared" ref="L13:L15" si="16">K13</f>
         <v>0</v>
       </c>
       <c r="M13" s="9">
@@ -27204,7 +27204,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" ref="P13:P27" si="17">O13</f>
+        <f t="shared" ref="P13:P15" si="17">O13</f>
         <v>0</v>
       </c>
       <c r="Q13" s="9">
@@ -27219,7 +27219,7 @@
         <v>0.5</v>
       </c>
       <c r="T13" s="8">
-        <f t="shared" ref="T13:T27" si="18">S13</f>
+        <f t="shared" ref="T13:T15" si="18">S13</f>
         <v>0.5</v>
       </c>
       <c r="U13" s="9">
@@ -27234,7 +27234,7 @@
         <v>1.7</v>
       </c>
       <c r="X13" s="8">
-        <f t="shared" ref="X13:X27" si="19">W13</f>
+        <f t="shared" ref="X13:X15" si="19">W13</f>
         <v>1.7</v>
       </c>
       <c r="Y13" s="9">
@@ -27249,7 +27249,7 @@
         <v>1</v>
       </c>
       <c r="AB13" s="8">
-        <f t="shared" ref="AB13:AB27" si="20">AA13</f>
+        <f t="shared" ref="AB13:AB15" si="20">AA13</f>
         <v>1</v>
       </c>
       <c r="AC13" s="9">
@@ -28519,7 +28519,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="9">
-        <f t="shared" ref="M27:M29" si="45">L19</f>
+        <f t="shared" ref="M27" si="45">L19</f>
         <v>0</v>
       </c>
       <c r="O27" s="5">
@@ -28531,7 +28531,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="9">
-        <f t="shared" ref="Q27:Q29" si="46">P19</f>
+        <f t="shared" ref="Q27" si="46">P19</f>
         <v>0</v>
       </c>
       <c r="R27" s="4">
@@ -28546,7 +28546,7 @@
         <v>25</v>
       </c>
       <c r="U27" s="9">
-        <f t="shared" ref="U27:U29" si="47">T19</f>
+        <f t="shared" ref="U27" si="47">T19</f>
         <v>25</v>
       </c>
       <c r="V27" s="4">
@@ -28561,7 +28561,7 @@
         <v>55</v>
       </c>
       <c r="Y27" s="9">
-        <f t="shared" ref="Y27:Y29" si="48">X19</f>
+        <f t="shared" ref="Y27" si="48">X19</f>
         <v>50</v>
       </c>
       <c r="Z27" s="4">
@@ -28576,7 +28576,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="9">
-        <f t="shared" ref="AC27:AC29" si="49">AB19</f>
+        <f t="shared" ref="AC27" si="49">AB19</f>
         <v>78</v>
       </c>
     </row>
@@ -29005,7 +29005,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="8">
-        <f t="shared" ref="L32:L39" si="61">K32</f>
+        <f t="shared" ref="L32:L33" si="61">K32</f>
         <v>0</v>
       </c>
       <c r="M32" s="9">
@@ -29017,7 +29017,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="8">
-        <f t="shared" ref="P32:P39" si="62">O32</f>
+        <f t="shared" ref="P32:P33" si="62">O32</f>
         <v>0</v>
       </c>
       <c r="Q32" s="9">
@@ -29032,7 +29032,7 @@
         <v>4</v>
       </c>
       <c r="T32" s="8">
-        <f t="shared" ref="T32:T39" si="63">S32</f>
+        <f t="shared" ref="T32:T33" si="63">S32</f>
         <v>4</v>
       </c>
       <c r="U32" s="9">
@@ -29047,7 +29047,7 @@
         <v>15</v>
       </c>
       <c r="X32" s="8">
-        <f t="shared" ref="X32:X39" si="64">W32</f>
+        <f t="shared" ref="X32:X33" si="64">W32</f>
         <v>15</v>
       </c>
       <c r="Y32" s="9">
@@ -29059,7 +29059,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="8">
-        <f t="shared" ref="AB32:AB39" si="65">AA32</f>
+        <f t="shared" ref="AB32:AB33" si="65">AA32</f>
         <v>0</v>
       </c>
       <c r="AC32" s="9">
@@ -29192,11 +29192,11 @@
         <v>5</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" ref="K34:K58" si="68">$C34*J34</f>
+        <f t="shared" ref="K34:K39" si="68">$C34*J34</f>
         <v>0.25</v>
       </c>
       <c r="L34" s="8">
-        <f t="shared" ref="L34:L37" si="69">$D34*K34</f>
+        <f t="shared" ref="L34" si="69">$D34*K34</f>
         <v>2.5</v>
       </c>
       <c r="M34" s="13">
@@ -29207,11 +29207,11 @@
         <v>3</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" ref="O34:O58" si="70">$C34*N34</f>
+        <f t="shared" ref="O34:O39" si="70">$C34*N34</f>
         <v>0.15000000000000002</v>
       </c>
       <c r="P34" s="8">
-        <f t="shared" ref="P34:P37" si="71">$D34*O34</f>
+        <f t="shared" ref="P34" si="71">$D34*O34</f>
         <v>1.5000000000000002</v>
       </c>
       <c r="Q34" s="13">
@@ -29222,11 +29222,11 @@
         <v>5</v>
       </c>
       <c r="S34" s="5">
-        <f t="shared" ref="S34:S58" si="72">$C34*R34</f>
+        <f t="shared" ref="S34:S39" si="72">$C34*R34</f>
         <v>0.25</v>
       </c>
       <c r="T34" s="8">
-        <f t="shared" ref="T34:T37" si="73">$D34*S34</f>
+        <f t="shared" ref="T34" si="73">$D34*S34</f>
         <v>2.5</v>
       </c>
       <c r="U34" s="13">
@@ -29237,11 +29237,11 @@
         <v>6</v>
       </c>
       <c r="W34" s="5">
-        <f t="shared" ref="W34:W58" si="74">$C34*V34</f>
+        <f t="shared" ref="W34:W39" si="74">$C34*V34</f>
         <v>0.30000000000000004</v>
       </c>
       <c r="X34" s="8">
-        <f t="shared" ref="X34:X37" si="75">$D34*W34</f>
+        <f t="shared" ref="X34" si="75">$D34*W34</f>
         <v>3.0000000000000004</v>
       </c>
       <c r="Y34" s="13">
@@ -29252,11 +29252,11 @@
         <v>5</v>
       </c>
       <c r="AA34" s="5">
-        <f t="shared" ref="AA34:AA58" si="76">$C34*Z34</f>
+        <f t="shared" ref="AA34:AA39" si="76">$C34*Z34</f>
         <v>0.25</v>
       </c>
       <c r="AB34" s="8">
-        <f t="shared" ref="AB34:AB37" si="77">$D34*AA34</f>
+        <f t="shared" ref="AB34" si="77">$D34*AA34</f>
         <v>2.5</v>
       </c>
       <c r="AC34" s="13">
@@ -29523,7 +29523,7 @@
         <v>0.1</v>
       </c>
       <c r="L37" s="8">
-        <f t="shared" ref="L37:L40" si="79">$D37*K37</f>
+        <f t="shared" ref="L37" si="79">$D37*K37</f>
         <v>1</v>
       </c>
       <c r="M37" s="13">
@@ -29535,7 +29535,7 @@
         <v>0</v>
       </c>
       <c r="P37" s="8">
-        <f t="shared" ref="P37:P40" si="80">$D37*O37</f>
+        <f t="shared" ref="P37" si="80">$D37*O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="13">
@@ -29550,7 +29550,7 @@
         <v>0.05</v>
       </c>
       <c r="T37" s="8">
-        <f t="shared" ref="T37:T40" si="81">$D37*S37</f>
+        <f t="shared" ref="T37" si="81">$D37*S37</f>
         <v>0.5</v>
       </c>
       <c r="U37" s="13">
@@ -29562,7 +29562,7 @@
         <v>0</v>
       </c>
       <c r="X37" s="8">
-        <f t="shared" ref="X37:X40" si="82">$D37*W37</f>
+        <f t="shared" ref="X37" si="82">$D37*W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="13">
@@ -29574,7 +29574,7 @@
         <v>0</v>
       </c>
       <c r="AB37" s="8">
-        <f t="shared" ref="AB37:AB40" si="83">$D37*AA37</f>
+        <f t="shared" ref="AB37" si="83">$D37*AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="13">
@@ -29923,75 +29923,75 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" ref="K41:K65" si="87">$C41*J41</f>
+        <f t="shared" ref="K41:K47" si="87">$C41*J41</f>
         <v>0</v>
       </c>
       <c r="L41" s="8">
-        <f t="shared" ref="L41:L45" si="88">$D41*K41</f>
+        <f t="shared" ref="L41" si="88">$D41*K41</f>
         <v>0</v>
       </c>
       <c r="M41" s="13">
-        <f t="shared" ref="M41:M52" si="89">$E41*L41</f>
+        <f t="shared" ref="M41" si="89">$E41*L41</f>
         <v>0</v>
       </c>
       <c r="N41" s="4">
         <v>1</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" ref="O41:O65" si="90">$C41*N41</f>
+        <f t="shared" ref="O41:O47" si="90">$C41*N41</f>
         <v>0.05</v>
       </c>
       <c r="P41" s="8">
-        <f t="shared" ref="P41:P45" si="91">$D41*O41</f>
+        <f t="shared" ref="P41" si="91">$D41*O41</f>
         <v>0.5</v>
       </c>
       <c r="Q41" s="13">
-        <f t="shared" ref="Q41:Q52" si="92">$E41*P41</f>
+        <f t="shared" ref="Q41" si="92">$E41*P41</f>
         <v>1.5</v>
       </c>
       <c r="R41" s="4">
         <v>0.01</v>
       </c>
       <c r="S41" s="5">
-        <f t="shared" ref="S41:S65" si="93">$C41*R41</f>
+        <f t="shared" ref="S41:S47" si="93">$C41*R41</f>
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="T41" s="8">
-        <f t="shared" ref="T41:T45" si="94">$D41*S41</f>
+        <f t="shared" ref="T41" si="94">$D41*S41</f>
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="U41" s="13">
-        <f t="shared" ref="U41:U52" si="95">$E41*T41</f>
+        <f t="shared" ref="U41" si="95">$E41*T41</f>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="V41" s="4">
         <v>0.4</v>
       </c>
       <c r="W41" s="5">
-        <f t="shared" ref="W41:W65" si="96">$C41*V41</f>
+        <f t="shared" ref="W41:W47" si="96">$C41*V41</f>
         <v>2.0000000000000004E-2</v>
       </c>
       <c r="X41" s="8">
-        <f t="shared" ref="X41:X45" si="97">$D41*W41</f>
+        <f t="shared" ref="X41" si="97">$D41*W41</f>
         <v>0.20000000000000004</v>
       </c>
       <c r="Y41" s="13">
-        <f t="shared" ref="Y41:Y52" si="98">$E41*X41</f>
+        <f t="shared" ref="Y41" si="98">$E41*X41</f>
         <v>0.60000000000000009</v>
       </c>
       <c r="Z41" s="4">
         <v>0.1</v>
       </c>
       <c r="AA41" s="5">
-        <f t="shared" ref="AA41:AA65" si="99">$C41*Z41</f>
+        <f t="shared" ref="AA41:AA47" si="99">$C41*Z41</f>
         <v>5.000000000000001E-3</v>
       </c>
       <c r="AB41" s="8">
-        <f t="shared" ref="AB41:AB45" si="100">$D41*AA41</f>
+        <f t="shared" ref="AB41" si="100">$D41*AA41</f>
         <v>5.000000000000001E-2</v>
       </c>
       <c r="AC41" s="13">
-        <f t="shared" ref="AC41:AC52" si="101">$E41*AB41</f>
+        <f t="shared" ref="AC41" si="101">$E41*AB41</f>
         <v>0.15000000000000002</v>
       </c>
     </row>
@@ -30245,7 +30245,7 @@
         <v>0</v>
       </c>
       <c r="L44" s="8">
-        <f t="shared" ref="L44:L48" si="102">$D44*K44</f>
+        <f t="shared" ref="L44:L45" si="102">$D44*K44</f>
         <v>0</v>
       </c>
       <c r="M44" s="13">
@@ -30260,7 +30260,7 @@
         <v>0.05</v>
       </c>
       <c r="P44" s="8">
-        <f t="shared" ref="P44:P48" si="103">$D44*O44</f>
+        <f t="shared" ref="P44:P45" si="103">$D44*O44</f>
         <v>0.5</v>
       </c>
       <c r="Q44" s="13">
@@ -30275,7 +30275,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="T44" s="8">
-        <f t="shared" ref="T44:T48" si="104">$D44*S44</f>
+        <f t="shared" ref="T44:T45" si="104">$D44*S44</f>
         <v>0.25</v>
       </c>
       <c r="U44" s="13">
@@ -30287,7 +30287,7 @@
         <v>0</v>
       </c>
       <c r="X44" s="8">
-        <f t="shared" ref="X44:X48" si="105">$D44*W44</f>
+        <f t="shared" ref="X44:X45" si="105">$D44*W44</f>
         <v>0</v>
       </c>
       <c r="Y44" s="13">
@@ -30302,7 +30302,7 @@
         <v>0.05</v>
       </c>
       <c r="AB44" s="8">
-        <f t="shared" ref="AB44:AB48" si="106">$D44*AA44</f>
+        <f t="shared" ref="AB44:AB45" si="106">$D44*AA44</f>
         <v>0.5</v>
       </c>
       <c r="AC44" s="13">
@@ -30353,7 +30353,7 @@
         <v>0</v>
       </c>
       <c r="M45" s="13">
-        <f t="shared" ref="M45:M56" si="107">$E45*L45</f>
+        <f t="shared" ref="M45" si="107">$E45*L45</f>
         <v>0</v>
       </c>
       <c r="N45" s="4">
@@ -30368,7 +30368,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="Q45" s="13">
-        <f t="shared" ref="Q45:Q56" si="108">$E45*P45</f>
+        <f t="shared" ref="Q45" si="108">$E45*P45</f>
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="R45" s="4">
@@ -30383,7 +30383,7 @@
         <v>0.01</v>
       </c>
       <c r="U45" s="13">
-        <f t="shared" ref="U45:U56" si="109">$E45*T45</f>
+        <f t="shared" ref="U45" si="109">$E45*T45</f>
         <v>0.03</v>
       </c>
       <c r="W45" s="5">
@@ -30395,7 +30395,7 @@
         <v>0</v>
       </c>
       <c r="Y45" s="13">
-        <f t="shared" ref="Y45:Y56" si="110">$E45*X45</f>
+        <f t="shared" ref="Y45" si="110">$E45*X45</f>
         <v>0</v>
       </c>
       <c r="Z45" s="4">
@@ -30410,7 +30410,7 @@
         <v>5.000000000000001E-2</v>
       </c>
       <c r="AC45" s="13">
-        <f t="shared" ref="AC45:AC56" si="111">$E45*AB45</f>
+        <f t="shared" ref="AC45" si="111">$E45*AB45</f>
         <v>0.15000000000000002</v>
       </c>
     </row>
@@ -30668,7 +30668,7 @@
         <v>0.5</v>
       </c>
       <c r="M48" s="13">
-        <f t="shared" ref="M48:M59" si="114">$E48*L48</f>
+        <f t="shared" ref="M48:M52" si="114">$E48*L48</f>
         <v>1</v>
       </c>
       <c r="O48" s="5">
@@ -30680,7 +30680,7 @@
         <v>0</v>
       </c>
       <c r="Q48" s="13">
-        <f t="shared" ref="Q48:Q59" si="116">$E48*P48</f>
+        <f t="shared" ref="Q48:Q52" si="116">$E48*P48</f>
         <v>0</v>
       </c>
       <c r="R48" s="4">
@@ -30695,7 +30695,7 @@
         <v>0.25</v>
       </c>
       <c r="U48" s="13">
-        <f t="shared" ref="U48:U59" si="118">$E48*T48</f>
+        <f t="shared" ref="U48:U52" si="118">$E48*T48</f>
         <v>0.5</v>
       </c>
       <c r="V48" s="4">
@@ -30710,7 +30710,7 @@
         <v>0.5</v>
       </c>
       <c r="Y48" s="13">
-        <f t="shared" ref="Y48:Y59" si="120">$E48*X48</f>
+        <f t="shared" ref="Y48:Y52" si="120">$E48*X48</f>
         <v>1</v>
       </c>
       <c r="Z48" s="4">
@@ -30725,7 +30725,7 @@
         <v>0.25</v>
       </c>
       <c r="AC48" s="13">
-        <f t="shared" ref="AC48:AC59" si="122">$E48*AB48</f>
+        <f t="shared" ref="AC48:AC52" si="122">$E48*AB48</f>
         <v>0.5</v>
       </c>
     </row>
@@ -30767,7 +30767,7 @@
         <v>50</v>
       </c>
       <c r="K49" s="5">
-        <f t="shared" ref="K49:K73" si="123">$C49*J49</f>
+        <f t="shared" ref="K49:K58" si="123">$C49*J49</f>
         <v>2.5</v>
       </c>
       <c r="L49" s="8">
@@ -30779,7 +30779,7 @@
         <v>50</v>
       </c>
       <c r="O49" s="5">
-        <f t="shared" ref="O49:O73" si="124">$C49*N49</f>
+        <f t="shared" ref="O49:O58" si="124">$C49*N49</f>
         <v>0</v>
       </c>
       <c r="P49" s="8">
@@ -30794,7 +30794,7 @@
         <v>30</v>
       </c>
       <c r="S49" s="5">
-        <f t="shared" ref="S49:S73" si="125">$C49*R49</f>
+        <f t="shared" ref="S49:S58" si="125">$C49*R49</f>
         <v>1.5</v>
       </c>
       <c r="T49" s="8">
@@ -30809,7 +30809,7 @@
         <v>40</v>
       </c>
       <c r="W49" s="5">
-        <f t="shared" ref="W49:W73" si="126">$C49*V49</f>
+        <f t="shared" ref="W49:W58" si="126">$C49*V49</f>
         <v>2</v>
       </c>
       <c r="X49" s="8">
@@ -30824,7 +30824,7 @@
         <v>15</v>
       </c>
       <c r="AA49" s="5">
-        <f t="shared" ref="AA49:AA73" si="127">$C49*Z49</f>
+        <f t="shared" ref="AA49:AA58" si="127">$C49*Z49</f>
         <v>0.75</v>
       </c>
       <c r="AB49" s="8">
@@ -31894,7 +31894,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="9">
-        <f t="shared" ref="M60:M78" si="140">L60</f>
+        <f t="shared" ref="M60:M77" si="140">L60</f>
         <v>0</v>
       </c>
       <c r="O60" s="5">
@@ -31906,7 +31906,7 @@
         <v>0</v>
       </c>
       <c r="Q60" s="9">
-        <f t="shared" ref="Q60:Q78" si="141">P60</f>
+        <f t="shared" ref="Q60:Q77" si="141">P60</f>
         <v>0</v>
       </c>
       <c r="R60" s="4">
@@ -31921,7 +31921,7 @@
         <v>2</v>
       </c>
       <c r="U60" s="9">
-        <f t="shared" ref="U60:U78" si="142">T60</f>
+        <f t="shared" ref="U60:U77" si="142">T60</f>
         <v>2</v>
       </c>
       <c r="W60" s="5">
@@ -31933,7 +31933,7 @@
         <v>0</v>
       </c>
       <c r="Y60" s="9">
-        <f t="shared" ref="Y60:Y78" si="143">X60</f>
+        <f t="shared" ref="Y60:Y77" si="143">X60</f>
         <v>0</v>
       </c>
       <c r="AA60" s="5">
@@ -31945,7 +31945,7 @@
         <v>0</v>
       </c>
       <c r="AC60" s="9">
-        <f t="shared" ref="AC60:AC78" si="144">AB60</f>
+        <f t="shared" ref="AC60:AC77" si="144">AB60</f>
         <v>0</v>
       </c>
     </row>
@@ -33558,7 +33558,7 @@
         <v>0</v>
       </c>
       <c r="M78" s="13">
-        <f t="shared" ref="M78:M82" si="160">$E78*L78</f>
+        <f t="shared" ref="M78" si="160">$E78*L78</f>
         <v>0</v>
       </c>
       <c r="O78" s="5">
@@ -33570,7 +33570,7 @@
         <v>0</v>
       </c>
       <c r="Q78" s="13">
-        <f t="shared" ref="Q78:Q82" si="162">$E78*P78</f>
+        <f t="shared" ref="Q78" si="162">$E78*P78</f>
         <v>0</v>
       </c>
       <c r="R78" s="4">
@@ -33585,7 +33585,7 @@
         <v>1</v>
       </c>
       <c r="U78" s="13">
-        <f t="shared" ref="U78:U82" si="164">$E78*T78</f>
+        <f t="shared" ref="U78" si="164">$E78*T78</f>
         <v>15</v>
       </c>
       <c r="W78" s="5">
@@ -33597,7 +33597,7 @@
         <v>0</v>
       </c>
       <c r="Y78" s="13">
-        <f t="shared" ref="Y78:Y82" si="166">$E78*X78</f>
+        <f t="shared" ref="Y78" si="166">$E78*X78</f>
         <v>0</v>
       </c>
       <c r="AA78" s="5">
@@ -33609,7 +33609,7 @@
         <v>0</v>
       </c>
       <c r="AC78" s="13">
-        <f t="shared" ref="AC78:AC82" si="168">$E78*AB78</f>
+        <f t="shared" ref="AC78" si="168">$E78*AB78</f>
         <v>0</v>
       </c>
     </row>
@@ -33750,11 +33750,11 @@
         <v>0.05</v>
       </c>
       <c r="L80" s="8">
-        <f t="shared" ref="L80:L82" si="170">$D80*K80</f>
+        <f t="shared" ref="L80" si="170">$D80*K80</f>
         <v>0.5</v>
       </c>
       <c r="M80" s="13">
-        <f t="shared" ref="M80:M84" si="171">$E80*L80</f>
+        <f t="shared" ref="M80" si="171">$E80*L80</f>
         <v>7.5</v>
       </c>
       <c r="N80" s="4">
@@ -33765,11 +33765,11 @@
         <v>0.125</v>
       </c>
       <c r="P80" s="8">
-        <f t="shared" ref="P80:P82" si="172">$D80*O80</f>
+        <f t="shared" ref="P80" si="172">$D80*O80</f>
         <v>1.25</v>
       </c>
       <c r="Q80" s="13">
-        <f t="shared" ref="Q80:Q84" si="173">$E80*P80</f>
+        <f t="shared" ref="Q80" si="173">$E80*P80</f>
         <v>18.75</v>
       </c>
       <c r="R80" s="4">
@@ -33780,11 +33780,11 @@
         <v>0.05</v>
       </c>
       <c r="T80" s="8">
-        <f t="shared" ref="T80:T82" si="174">$D80*S80</f>
+        <f t="shared" ref="T80" si="174">$D80*S80</f>
         <v>0.5</v>
       </c>
       <c r="U80" s="13">
-        <f t="shared" ref="U80:U84" si="175">$E80*T80</f>
+        <f t="shared" ref="U80" si="175">$E80*T80</f>
         <v>7.5</v>
       </c>
       <c r="V80" s="4">
@@ -33795,11 +33795,11 @@
         <v>7.5000000000000011E-2</v>
       </c>
       <c r="X80" s="8">
-        <f t="shared" ref="X80:X82" si="176">$D80*W80</f>
+        <f t="shared" ref="X80" si="176">$D80*W80</f>
         <v>0.75000000000000011</v>
       </c>
       <c r="Y80" s="13">
-        <f t="shared" ref="Y80:Y84" si="177">$E80*X80</f>
+        <f t="shared" ref="Y80" si="177">$E80*X80</f>
         <v>11.250000000000002</v>
       </c>
       <c r="Z80" s="4">
@@ -33810,11 +33810,11 @@
         <v>0.1</v>
       </c>
       <c r="AB80" s="8">
-        <f t="shared" ref="AB80:AB82" si="178">$D80*AA80</f>
+        <f t="shared" ref="AB80" si="178">$D80*AA80</f>
         <v>1</v>
       </c>
       <c r="AC80" s="13">
-        <f t="shared" ref="AC80:AC84" si="179">$E80*AB80</f>
+        <f t="shared" ref="AC80" si="179">$E80*AB80</f>
         <v>15</v>
       </c>
     </row>
@@ -33964,11 +33964,11 @@
         <v>0</v>
       </c>
       <c r="L82" s="8">
-        <f t="shared" ref="L82:L84" si="180">$D82*K82</f>
+        <f t="shared" ref="L82" si="180">$D82*K82</f>
         <v>0</v>
       </c>
       <c r="M82" s="13">
-        <f t="shared" ref="M82:M86" si="181">$E82*L82</f>
+        <f t="shared" ref="M82" si="181">$E82*L82</f>
         <v>0</v>
       </c>
       <c r="O82" s="5">
@@ -33976,11 +33976,11 @@
         <v>0</v>
       </c>
       <c r="P82" s="8">
-        <f t="shared" ref="P82:P84" si="182">$D82*O82</f>
+        <f t="shared" ref="P82" si="182">$D82*O82</f>
         <v>0</v>
       </c>
       <c r="Q82" s="13">
-        <f t="shared" ref="Q82:Q86" si="183">$E82*P82</f>
+        <f t="shared" ref="Q82" si="183">$E82*P82</f>
         <v>0</v>
       </c>
       <c r="R82" s="4">
@@ -33991,11 +33991,11 @@
         <v>0.125</v>
       </c>
       <c r="T82" s="8">
-        <f t="shared" ref="T82:T84" si="184">$D82*S82</f>
+        <f t="shared" ref="T82" si="184">$D82*S82</f>
         <v>1.25</v>
       </c>
       <c r="U82" s="13">
-        <f t="shared" ref="U82:U86" si="185">$E82*T82</f>
+        <f t="shared" ref="U82" si="185">$E82*T82</f>
         <v>18.75</v>
       </c>
       <c r="V82" s="4">
@@ -34006,11 +34006,11 @@
         <v>0.05</v>
       </c>
       <c r="X82" s="8">
-        <f t="shared" ref="X82:X84" si="186">$D82*W82</f>
+        <f t="shared" ref="X82" si="186">$D82*W82</f>
         <v>0.5</v>
       </c>
       <c r="Y82" s="13">
-        <f t="shared" ref="Y82:Y86" si="187">$E82*X82</f>
+        <f t="shared" ref="Y82" si="187">$E82*X82</f>
         <v>7.5</v>
       </c>
       <c r="AA82" s="5">
@@ -34018,11 +34018,11 @@
         <v>0</v>
       </c>
       <c r="AB82" s="8">
-        <f t="shared" ref="AB82:AB84" si="188">$D82*AA82</f>
+        <f t="shared" ref="AB82" si="188">$D82*AA82</f>
         <v>0</v>
       </c>
       <c r="AC82" s="13">
-        <f t="shared" ref="AC82:AC86" si="189">$E82*AB82</f>
+        <f t="shared" ref="AC82" si="189">$E82*AB82</f>
         <v>0</v>
       </c>
     </row>
@@ -39859,7 +39859,7 @@
       </c>
       <c r="AR20">
         <f>'11_Fire_LowSeverity'!X20</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="AS20">
         <f>'11_Fire_LowSeverity'!Y20</f>
@@ -41085,7 +41085,7 @@
       </c>
       <c r="AQ25">
         <f>'11_Fire_LowSeverity'!W25</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="AR25">
         <f>'11_Fire_LowSeverity'!X25</f>
@@ -41831,7 +41831,7 @@
       </c>
       <c r="AS28">
         <f>'11_Fire_LowSeverity'!Y28</f>
-        <v>19.5</v>
+        <v>24.5</v>
       </c>
       <c r="AT28">
         <f>'12_Fire_ModSeverity'!W28</f>

</xml_diff>

<commit_message>
Fixed errors in low and mod severity expected values
</commit_message>
<xml_diff>
--- a/specifications/1_Fire/ScriptRules_Fire.xlsx
+++ b/specifications/1_Fire/ScriptRules_Fire.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -1553,7 +1553,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1682,6 +1682,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="20% - Accent1" xfId="2" builtinId="30"/>
@@ -2524,24 +2536,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K951"/>
+  <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="101.28515625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="28" customWidth="1"/>
-    <col min="3" max="3" width="29.85546875" style="13" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" style="17" customWidth="1"/>
-    <col min="5" max="5" width="32.28515625" style="18" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="33" style="17" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="18" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="33.140625" style="17" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" style="18" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="101.28515625" style="61" customWidth="1"/>
+    <col min="2" max="2" width="28" style="44" customWidth="1"/>
+    <col min="3" max="3" width="29.85546875" style="53" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="54" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" style="55" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="53" customWidth="1"/>
+    <col min="7" max="7" width="33" style="54" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="55" customWidth="1"/>
+    <col min="9" max="9" width="20.42578125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="33.140625" style="54" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" style="55" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="61"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" customFormat="1" x14ac:dyDescent="0.25">
@@ -2576,7 +2590,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>108</v>
       </c>
@@ -2586,28 +2600,41 @@
       <c r="C2" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D2" s="17"/>
+      <c r="E2" s="18"/>
       <c r="F2" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H2" s="18"/>
       <c r="I2" s="13" t="s">
         <v>5</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K2" s="18"/>
+    </row>
+    <row r="3" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>103</v>
       </c>
       <c r="B3" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C3" s="13"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>105</v>
       </c>
@@ -2617,22 +2644,37 @@
       <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
+      <c r="D4" s="17"/>
+      <c r="E4" s="18"/>
       <c r="F4" s="13" t="s">
         <v>16</v>
       </c>
+      <c r="G4" s="17"/>
+      <c r="H4" s="18"/>
       <c r="I4" s="13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J4" s="17"/>
+      <c r="K4" s="18"/>
+    </row>
+    <row r="5" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="13"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="18"/>
+    </row>
+    <row r="6" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>106</v>
       </c>
@@ -2642,20 +2684,24 @@
       <c r="C6" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
       <c r="F6" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H6" s="18"/>
       <c r="I6" s="13" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>107</v>
       </c>
@@ -2665,28 +2711,41 @@
       <c r="C7" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="18"/>
       <c r="F7" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H7" s="18"/>
       <c r="I7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
         <v>98</v>
       </c>
       <c r="B8" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C8" s="13"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="18"/>
+    </row>
+    <row r="9" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
         <v>100</v>
       </c>
@@ -2696,22 +2755,37 @@
       <c r="C9" s="13" t="s">
         <v>1</v>
       </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18"/>
       <c r="F9" s="13" t="s">
         <v>16</v>
       </c>
+      <c r="G9" s="17"/>
+      <c r="H9" s="18"/>
       <c r="I9" s="13" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="17"/>
+      <c r="K9" s="18"/>
+    </row>
+    <row r="10" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
         <v>99</v>
       </c>
       <c r="B10" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C10" s="13"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="18"/>
+    </row>
+    <row r="11" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
         <v>101</v>
       </c>
@@ -2721,20 +2795,24 @@
       <c r="C11" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D11" s="17"/>
+      <c r="E11" s="18"/>
       <c r="F11" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H11" s="18"/>
       <c r="I11" s="13" t="s">
         <v>5</v>
       </c>
       <c r="J11" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="18"/>
+    </row>
+    <row r="12" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
         <v>102</v>
       </c>
@@ -2744,50 +2822,79 @@
       <c r="C12" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D12" s="17"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="13" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H12" s="18"/>
       <c r="I12" s="13" t="s">
         <v>5</v>
       </c>
       <c r="J12" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="18"/>
+    </row>
+    <row r="13" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
         <v>109</v>
       </c>
       <c r="B13" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="13"/>
+      <c r="D13" s="17"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="17"/>
+      <c r="K13" s="18"/>
+    </row>
+    <row r="14" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
         <v>111</v>
       </c>
       <c r="B14" t="s">
         <v>290</v>
       </c>
+      <c r="C14" s="13"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="18"/>
       <c r="F14" s="13" t="s">
         <v>19</v>
       </c>
+      <c r="G14" s="17"/>
+      <c r="H14" s="18"/>
       <c r="I14" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J14" s="17"/>
+      <c r="K14" s="18"/>
+    </row>
+    <row r="15" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>110</v>
       </c>
       <c r="B15" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C15" s="13"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="18"/>
+    </row>
+    <row r="16" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
         <v>112</v>
       </c>
@@ -2797,20 +2904,24 @@
       <c r="C16" s="13" t="s">
         <v>2</v>
       </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="18"/>
       <c r="F16" s="13" t="s">
         <v>17</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H16" s="18"/>
       <c r="I16" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J16" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="18"/>
+    </row>
+    <row r="17" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
         <v>113</v>
       </c>
@@ -2820,38 +2931,45 @@
       <c r="C17" s="13" t="s">
         <v>2</v>
       </c>
+      <c r="D17" s="17"/>
+      <c r="E17" s="18"/>
       <c r="F17" s="13" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>0</v>
       </c>
+      <c r="H17" s="18"/>
       <c r="I17" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J17" s="17" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K17" s="18"/>
+    </row>
+    <row r="18" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
         <v>84</v>
       </c>
       <c r="B18" t="s">
         <v>294</v>
       </c>
+      <c r="C18" s="13"/>
       <c r="D18" s="14" t="s">
         <v>420</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>407</v>
       </c>
+      <c r="F18" s="13"/>
       <c r="G18" s="14" t="s">
         <v>420</v>
       </c>
       <c r="H18" s="15" t="s">
         <v>407</v>
       </c>
+      <c r="I18" s="13"/>
       <c r="J18" s="14" t="s">
         <v>419</v>
       </c>
@@ -2859,25 +2977,28 @@
         <v>407</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="16" t="s">
         <v>85</v>
       </c>
       <c r="B19" t="s">
         <v>295</v>
       </c>
+      <c r="C19" s="13"/>
       <c r="D19" s="14" t="s">
         <v>405</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>407</v>
       </c>
+      <c r="F19" s="13"/>
       <c r="G19" s="14" t="s">
         <v>405</v>
       </c>
       <c r="H19" s="15" t="s">
         <v>407</v>
       </c>
+      <c r="I19" s="13"/>
       <c r="J19" s="14" t="s">
         <v>405</v>
       </c>
@@ -2885,25 +3006,28 @@
         <v>407</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="16" t="s">
         <v>86</v>
       </c>
       <c r="B20" t="s">
         <v>296</v>
       </c>
+      <c r="C20" s="13"/>
       <c r="D20" s="14" t="s">
         <v>406</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>407</v>
       </c>
+      <c r="F20" s="13"/>
       <c r="G20" s="14" t="s">
         <v>406</v>
       </c>
       <c r="H20" s="15" t="s">
         <v>407</v>
       </c>
+      <c r="I20" s="13"/>
       <c r="J20" s="14" t="s">
         <v>406</v>
       </c>
@@ -2911,7 +3035,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="16" t="s">
         <v>89</v>
       </c>
@@ -2924,6 +3048,7 @@
       <c r="D21" s="14" t="s">
         <v>407</v>
       </c>
+      <c r="E21" s="18"/>
       <c r="F21" s="13" t="s">
         <v>398</v>
       </c>
@@ -2943,7 +3068,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="16" t="s">
         <v>87</v>
       </c>
@@ -2956,6 +3081,7 @@
       <c r="D22" s="14" t="s">
         <v>407</v>
       </c>
+      <c r="E22" s="18"/>
       <c r="F22" s="13" t="s">
         <v>399</v>
       </c>
@@ -2975,7 +3101,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>88</v>
       </c>
@@ -2988,6 +3114,7 @@
       <c r="D23" s="14" t="s">
         <v>407</v>
       </c>
+      <c r="E23" s="18"/>
       <c r="F23" s="13" t="s">
         <v>400</v>
       </c>
@@ -3007,7 +3134,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="16" t="s">
         <v>90</v>
       </c>
@@ -3020,6 +3147,7 @@
       <c r="D24" s="14" t="s">
         <v>407</v>
       </c>
+      <c r="E24" s="18"/>
       <c r="F24" s="13" t="s">
         <v>413</v>
       </c>
@@ -3039,7 +3167,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="16" t="s">
         <v>91</v>
       </c>
@@ -3052,6 +3180,7 @@
       <c r="D25" s="14" t="s">
         <v>407</v>
       </c>
+      <c r="E25" s="18"/>
       <c r="F25" s="13" t="s">
         <v>414</v>
       </c>
@@ -3071,25 +3200,28 @@
         <v>407</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="16" t="s">
         <v>92</v>
       </c>
       <c r="B26" t="s">
         <v>302</v>
       </c>
+      <c r="C26" s="13"/>
       <c r="D26" s="14" t="s">
         <v>408</v>
       </c>
       <c r="E26" s="20" t="s">
         <v>403</v>
       </c>
+      <c r="F26" s="13"/>
       <c r="G26" s="14" t="s">
         <v>408</v>
       </c>
       <c r="H26" s="20" t="s">
         <v>403</v>
       </c>
+      <c r="I26" s="13"/>
       <c r="J26" s="14" t="s">
         <v>408</v>
       </c>
@@ -3097,25 +3229,28 @@
         <v>403</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="16" t="s">
         <v>93</v>
       </c>
       <c r="B27" t="s">
         <v>303</v>
       </c>
+      <c r="C27" s="13"/>
       <c r="D27" s="14" t="s">
         <v>409</v>
       </c>
       <c r="E27" s="20" t="s">
         <v>404</v>
       </c>
+      <c r="F27" s="13"/>
       <c r="G27" s="14" t="s">
         <v>409</v>
       </c>
       <c r="H27" s="20" t="s">
         <v>404</v>
       </c>
+      <c r="I27" s="13"/>
       <c r="J27" s="14" t="s">
         <v>409</v>
       </c>
@@ -3123,25 +3258,28 @@
         <v>404</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="16" t="s">
         <v>94</v>
       </c>
       <c r="B28" t="s">
         <v>304</v>
       </c>
+      <c r="C28" s="13"/>
       <c r="D28" s="14" t="s">
         <v>410</v>
       </c>
       <c r="E28" s="20" t="s">
         <v>410</v>
       </c>
+      <c r="F28" s="13"/>
       <c r="G28" s="14" t="s">
         <v>410</v>
       </c>
       <c r="H28" s="20" t="s">
         <v>410</v>
       </c>
+      <c r="I28" s="13"/>
       <c r="J28" s="14" t="s">
         <v>410</v>
       </c>
@@ -3149,25 +3287,28 @@
         <v>410</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16" t="s">
         <v>95</v>
       </c>
       <c r="B29" t="s">
         <v>305</v>
       </c>
+      <c r="C29" s="13"/>
       <c r="D29" s="14" t="s">
         <v>411</v>
       </c>
       <c r="E29" s="20" t="s">
         <v>411</v>
       </c>
+      <c r="F29" s="13"/>
       <c r="G29" s="14" t="s">
         <v>411</v>
       </c>
       <c r="H29" s="20" t="s">
         <v>411</v>
       </c>
+      <c r="I29" s="13"/>
       <c r="J29" s="14" t="s">
         <v>411</v>
       </c>
@@ -3175,25 +3316,28 @@
         <v>411</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="16" t="s">
         <v>96</v>
       </c>
       <c r="B30" t="s">
         <v>306</v>
       </c>
+      <c r="C30" s="13"/>
       <c r="D30" s="14" t="s">
         <v>411</v>
       </c>
       <c r="E30" s="20" t="s">
         <v>411</v>
       </c>
+      <c r="F30" s="13"/>
       <c r="G30" s="14" t="s">
         <v>411</v>
       </c>
       <c r="H30" s="20" t="s">
         <v>411</v>
       </c>
+      <c r="I30" s="13"/>
       <c r="J30" s="14" t="s">
         <v>411</v>
       </c>
@@ -3201,25 +3345,28 @@
         <v>411</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="16" t="s">
         <v>97</v>
       </c>
       <c r="B31" t="s">
         <v>307</v>
       </c>
+      <c r="C31" s="13"/>
       <c r="D31" s="14" t="s">
         <v>412</v>
       </c>
       <c r="E31" s="20" t="s">
         <v>412</v>
       </c>
+      <c r="F31" s="13"/>
       <c r="G31" s="14" t="s">
         <v>412</v>
       </c>
       <c r="H31" s="20" t="s">
         <v>412</v>
       </c>
+      <c r="I31" s="13"/>
       <c r="J31" s="14" t="s">
         <v>412</v>
       </c>
@@ -3227,23 +3374,41 @@
         <v>412</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="16" t="s">
         <v>82</v>
       </c>
       <c r="B32" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="13"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="18"/>
+    </row>
+    <row r="33" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16" t="s">
         <v>83</v>
       </c>
       <c r="B33" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="13"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="18"/>
+      <c r="F33" s="13"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="18"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="18"/>
+    </row>
+    <row r="34" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="16" t="s">
         <v>148</v>
       </c>
@@ -3278,7 +3443,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16" t="s">
         <v>149</v>
       </c>
@@ -3313,7 +3478,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="16" t="s">
         <v>150</v>
       </c>
@@ -3344,7 +3509,7 @@
       </c>
       <c r="K36" s="15"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="16" t="s">
         <v>151</v>
       </c>
@@ -3379,7 +3544,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16" t="s">
         <v>152</v>
       </c>
@@ -3414,7 +3579,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="16" t="s">
         <v>153</v>
       </c>
@@ -3445,7 +3610,7 @@
       </c>
       <c r="K39" s="15"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="16" t="s">
         <v>126</v>
       </c>
@@ -3458,6 +3623,7 @@
       <c r="D40" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E40" s="18"/>
       <c r="F40" s="13" t="s">
         <v>5</v>
       </c>
@@ -3473,7 +3639,7 @@
       </c>
       <c r="K40" s="15"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="16" t="s">
         <v>127</v>
       </c>
@@ -3486,6 +3652,7 @@
       <c r="D41" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E41" s="18"/>
       <c r="F41" s="13" t="s">
         <v>5</v>
       </c>
@@ -3501,7 +3668,7 @@
       </c>
       <c r="K41" s="15"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="16" t="s">
         <v>128</v>
       </c>
@@ -3514,6 +3681,7 @@
       <c r="D42" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E42" s="18"/>
       <c r="F42" s="13" t="s">
         <v>5</v>
       </c>
@@ -3529,7 +3697,7 @@
       </c>
       <c r="K42" s="15"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="16" t="s">
         <v>129</v>
       </c>
@@ -3542,6 +3710,7 @@
       <c r="D43" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E43" s="18"/>
       <c r="F43" s="13" t="s">
         <v>5</v>
       </c>
@@ -3557,7 +3726,7 @@
       </c>
       <c r="K43" s="15"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="16" t="s">
         <v>130</v>
       </c>
@@ -3570,6 +3739,7 @@
       <c r="D44" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E44" s="18"/>
       <c r="F44" s="13" t="s">
         <v>5</v>
       </c>
@@ -3585,7 +3755,7 @@
       </c>
       <c r="K44" s="15"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="16" t="s">
         <v>131</v>
       </c>
@@ -3598,6 +3768,7 @@
       <c r="D45" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E45" s="18"/>
       <c r="F45" s="13" t="s">
         <v>5</v>
       </c>
@@ -3613,7 +3784,7 @@
       </c>
       <c r="K45" s="15"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="16" t="s">
         <v>132</v>
       </c>
@@ -3626,6 +3797,7 @@
       <c r="D46" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E46" s="18"/>
       <c r="F46" s="13" t="s">
         <v>5</v>
       </c>
@@ -3641,7 +3813,7 @@
       </c>
       <c r="K46" s="15"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="16" t="s">
         <v>133</v>
       </c>
@@ -3654,6 +3826,7 @@
       <c r="D47" s="14" t="s">
         <v>391</v>
       </c>
+      <c r="E47" s="18"/>
       <c r="F47" s="13" t="s">
         <v>5</v>
       </c>
@@ -3669,7 +3842,7 @@
       </c>
       <c r="K47" s="15"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="16" t="s">
         <v>154</v>
       </c>
@@ -3704,7 +3877,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16" t="s">
         <v>155</v>
       </c>
@@ -3739,7 +3912,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="16" t="s">
         <v>159</v>
       </c>
@@ -3774,7 +3947,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="16" t="s">
         <v>160</v>
       </c>
@@ -3809,7 +3982,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="16" t="s">
         <v>161</v>
       </c>
@@ -3844,7 +4017,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="16" t="s">
         <v>227</v>
       </c>
@@ -3879,7 +4052,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="16" t="s">
         <v>228</v>
       </c>
@@ -3914,7 +4087,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
         <v>229</v>
       </c>
@@ -3949,7 +4122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="16" t="s">
         <v>230</v>
       </c>
@@ -3984,7 +4157,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="16" t="s">
         <v>231</v>
       </c>
@@ -4019,7 +4192,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="16" t="s">
         <v>232</v>
       </c>
@@ -4054,31 +4227,58 @@
         <v>426</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="16" t="s">
         <v>168</v>
       </c>
       <c r="B59" t="s">
         <v>335</v>
       </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C59" s="13"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="18"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="18"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="17"/>
+      <c r="K59" s="18"/>
+    </row>
+    <row r="60" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="16" t="s">
         <v>169</v>
       </c>
       <c r="B60" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C60" s="13"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="18"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="17"/>
+      <c r="K60" s="18"/>
+    </row>
+    <row r="61" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="16" t="s">
         <v>170</v>
       </c>
       <c r="B61" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C61" s="13"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="18"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="17"/>
+      <c r="K61" s="18"/>
+    </row>
+    <row r="62" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="16" t="s">
         <v>165</v>
       </c>
@@ -4088,14 +4288,20 @@
       <c r="C62" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D62" s="17"/>
+      <c r="E62" s="18"/>
       <c r="F62" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="18"/>
       <c r="I62" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J62" s="17"/>
+      <c r="K62" s="18"/>
+    </row>
+    <row r="63" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="16" t="s">
         <v>166</v>
       </c>
@@ -4105,14 +4311,20 @@
       <c r="C63" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D63" s="17"/>
+      <c r="E63" s="18"/>
       <c r="F63" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="G63" s="17"/>
+      <c r="H63" s="18"/>
       <c r="I63" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J63" s="17"/>
+      <c r="K63" s="18"/>
+    </row>
+    <row r="64" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="16" t="s">
         <v>167</v>
       </c>
@@ -4122,14 +4334,20 @@
       <c r="C64" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D64" s="17"/>
+      <c r="E64" s="18"/>
       <c r="F64" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="G64" s="17"/>
+      <c r="H64" s="18"/>
       <c r="I64" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J64" s="17"/>
+      <c r="K64" s="18"/>
+    </row>
+    <row r="65" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="16" t="s">
         <v>162</v>
       </c>
@@ -4139,14 +4357,20 @@
       <c r="C65" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D65" s="17"/>
+      <c r="E65" s="18"/>
       <c r="F65" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="G65" s="17"/>
+      <c r="H65" s="18"/>
       <c r="I65" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J65" s="17"/>
+      <c r="K65" s="18"/>
+    </row>
+    <row r="66" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="16" t="s">
         <v>163</v>
       </c>
@@ -4156,14 +4380,20 @@
       <c r="C66" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D66" s="17"/>
+      <c r="E66" s="18"/>
       <c r="F66" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="G66" s="17"/>
+      <c r="H66" s="18"/>
       <c r="I66" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J66" s="17"/>
+      <c r="K66" s="18"/>
+    </row>
+    <row r="67" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16" t="s">
         <v>164</v>
       </c>
@@ -4173,14 +4403,20 @@
       <c r="C67" s="13" t="s">
         <v>0</v>
       </c>
+      <c r="D67" s="17"/>
+      <c r="E67" s="18"/>
       <c r="F67" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="G67" s="17"/>
+      <c r="H67" s="18"/>
       <c r="I67" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J67" s="17"/>
+      <c r="K67" s="18"/>
+    </row>
+    <row r="68" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="16" t="s">
         <v>156</v>
       </c>
@@ -4190,14 +4426,20 @@
       <c r="C68" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="D68" s="17"/>
+      <c r="E68" s="18"/>
       <c r="F68" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G68" s="17"/>
+      <c r="H68" s="18"/>
       <c r="I68" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J68" s="17"/>
+      <c r="K68" s="18"/>
+    </row>
+    <row r="69" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16" t="s">
         <v>157</v>
       </c>
@@ -4207,14 +4449,20 @@
       <c r="C69" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="D69" s="17"/>
+      <c r="E69" s="18"/>
       <c r="F69" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G69" s="17"/>
+      <c r="H69" s="18"/>
       <c r="I69" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J69" s="17"/>
+      <c r="K69" s="18"/>
+    </row>
+    <row r="70" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="16" t="s">
         <v>158</v>
       </c>
@@ -4224,70 +4472,139 @@
       <c r="C70" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="D70" s="17"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G70" s="17"/>
+      <c r="H70" s="18"/>
       <c r="I70" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J70" s="17"/>
+      <c r="K70" s="18"/>
+    </row>
+    <row r="71" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="16" t="s">
         <v>134</v>
       </c>
       <c r="B71" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C71" s="13"/>
+      <c r="D71" s="17"/>
+      <c r="E71" s="18"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="18"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="17"/>
+      <c r="K71" s="18"/>
+    </row>
+    <row r="72" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="16" t="s">
         <v>135</v>
       </c>
       <c r="B72" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C72" s="13"/>
+      <c r="D72" s="17"/>
+      <c r="E72" s="18"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="18"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="17"/>
+      <c r="K72" s="18"/>
+    </row>
+    <row r="73" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="16" t="s">
         <v>136</v>
       </c>
       <c r="B73" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C73" s="13"/>
+      <c r="D73" s="17"/>
+      <c r="E73" s="18"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="18"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="17"/>
+      <c r="K73" s="18"/>
+    </row>
+    <row r="74" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="16" t="s">
         <v>137</v>
       </c>
       <c r="B74" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C74" s="13"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="18"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="18"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="17"/>
+      <c r="K74" s="18"/>
+    </row>
+    <row r="75" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="16" t="s">
         <v>138</v>
       </c>
       <c r="B75" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C75" s="13"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="18"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="17"/>
+      <c r="K75" s="18"/>
+    </row>
+    <row r="76" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="16" t="s">
         <v>139</v>
       </c>
       <c r="B76" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C76" s="13"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="18"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="17"/>
+      <c r="K76" s="18"/>
+    </row>
+    <row r="77" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="16" t="s">
         <v>140</v>
       </c>
       <c r="B77" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C77" s="13"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="18"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="17"/>
+      <c r="K77" s="18"/>
+    </row>
+    <row r="78" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="16" t="s">
         <v>141</v>
       </c>
@@ -4297,6 +4614,7 @@
       <c r="C78" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="D78" s="17"/>
       <c r="E78" s="20" t="s">
         <v>24</v>
       </c>
@@ -4319,7 +4637,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="16" t="s">
         <v>142</v>
       </c>
@@ -4329,6 +4647,7 @@
       <c r="C79" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="D79" s="17"/>
       <c r="E79" s="20" t="s">
         <v>24</v>
       </c>
@@ -4351,7 +4670,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="16" t="s">
         <v>143</v>
       </c>
@@ -4364,6 +4683,7 @@
       <c r="D80" s="23" t="s">
         <v>24</v>
       </c>
+      <c r="E80" s="18"/>
       <c r="F80" s="13" t="s">
         <v>5</v>
       </c>
@@ -4383,7 +4703,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="16" t="s">
         <v>144</v>
       </c>
@@ -4396,6 +4716,7 @@
       <c r="D81" s="14" t="s">
         <v>24</v>
       </c>
+      <c r="E81" s="18"/>
       <c r="F81" s="13" t="s">
         <v>5</v>
       </c>
@@ -4415,7 +4736,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="16" t="s">
         <v>145</v>
       </c>
@@ -4425,6 +4746,7 @@
       <c r="C82" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="D82" s="17"/>
       <c r="E82" s="20" t="s">
         <v>24</v>
       </c>
@@ -4447,7 +4769,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="16" t="s">
         <v>146</v>
       </c>
@@ -4457,6 +4779,7 @@
       <c r="C83" s="13" t="s">
         <v>4</v>
       </c>
+      <c r="D83" s="17"/>
       <c r="E83" s="20" t="s">
         <v>24</v>
       </c>
@@ -4479,7 +4802,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="16" t="s">
         <v>119</v>
       </c>
@@ -4490,14 +4813,19 @@
         <v>4</v>
       </c>
       <c r="D84" s="14"/>
+      <c r="E84" s="18"/>
       <c r="F84" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G84" s="17"/>
+      <c r="H84" s="18"/>
       <c r="I84" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J84" s="17"/>
+      <c r="K84" s="18"/>
+    </row>
+    <row r="85" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="16" t="s">
         <v>120</v>
       </c>
@@ -4508,14 +4836,19 @@
         <v>4</v>
       </c>
       <c r="D85" s="14"/>
+      <c r="E85" s="18"/>
       <c r="F85" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G85" s="17"/>
+      <c r="H85" s="18"/>
       <c r="I85" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J85" s="17"/>
+      <c r="K85" s="18"/>
+    </row>
+    <row r="86" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="16" t="s">
         <v>121</v>
       </c>
@@ -4526,14 +4859,19 @@
         <v>4</v>
       </c>
       <c r="D86" s="14"/>
+      <c r="E86" s="18"/>
       <c r="F86" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G86" s="17"/>
+      <c r="H86" s="18"/>
       <c r="I86" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J86" s="17"/>
+      <c r="K86" s="18"/>
+    </row>
+    <row r="87" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="16" t="s">
         <v>122</v>
       </c>
@@ -4544,14 +4882,19 @@
         <v>4</v>
       </c>
       <c r="D87" s="14"/>
+      <c r="E87" s="18"/>
       <c r="F87" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G87" s="17"/>
+      <c r="H87" s="18"/>
       <c r="I87" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J87" s="17"/>
+      <c r="K87" s="18"/>
+    </row>
+    <row r="88" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="16" t="s">
         <v>116</v>
       </c>
@@ -4562,14 +4905,19 @@
         <v>4</v>
       </c>
       <c r="D88" s="14"/>
+      <c r="E88" s="18"/>
       <c r="F88" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G88" s="17"/>
+      <c r="H88" s="18"/>
       <c r="I88" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J88" s="17"/>
+      <c r="K88" s="18"/>
+    </row>
+    <row r="89" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16" t="s">
         <v>117</v>
       </c>
@@ -4580,14 +4928,19 @@
         <v>4</v>
       </c>
       <c r="D89" s="14"/>
+      <c r="E89" s="18"/>
       <c r="F89" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G89" s="17"/>
+      <c r="H89" s="18"/>
       <c r="I89" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J89" s="17"/>
+      <c r="K89" s="18"/>
+    </row>
+    <row r="90" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="16" t="s">
         <v>118</v>
       </c>
@@ -4598,14 +4951,19 @@
         <v>4</v>
       </c>
       <c r="D90" s="14"/>
+      <c r="E90" s="18"/>
       <c r="F90" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G90" s="17"/>
+      <c r="H90" s="18"/>
       <c r="I90" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J90" s="17"/>
+      <c r="K90" s="18"/>
+    </row>
+    <row r="91" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="16" t="s">
         <v>123</v>
       </c>
@@ -4616,14 +4974,19 @@
         <v>4</v>
       </c>
       <c r="D91" s="14"/>
+      <c r="E91" s="18"/>
       <c r="F91" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G91" s="17"/>
+      <c r="H91" s="18"/>
       <c r="I91" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J91" s="17"/>
+      <c r="K91" s="18"/>
+    </row>
+    <row r="92" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="16" t="s">
         <v>124</v>
       </c>
@@ -4634,889 +4997,41 @@
         <v>4</v>
       </c>
       <c r="D92" s="14"/>
+      <c r="E92" s="18"/>
       <c r="F92" s="13" t="s">
         <v>5</v>
       </c>
+      <c r="G92" s="17"/>
+      <c r="H92" s="18"/>
       <c r="I92" s="13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="16" t="s">
+      <c r="J92" s="17"/>
+      <c r="K92" s="18"/>
+    </row>
+    <row r="93" spans="1:11" s="60" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="58" t="s">
         <v>125</v>
       </c>
       <c r="B93" t="s">
         <v>366</v>
       </c>
-      <c r="C93" s="13" t="s">
+      <c r="C93" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="D93" s="14"/>
-      <c r="F93" s="13" t="s">
+      <c r="D93" s="59"/>
+      <c r="E93" s="49"/>
+      <c r="F93" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="I93" s="13" t="s">
+      <c r="G93" s="48"/>
+      <c r="H93" s="49"/>
+      <c r="I93" s="47" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="94" spans="1:11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" spans="1:11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" spans="1:11" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="104" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="105" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="106" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="107" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="108" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="109" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="110" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="111" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="112" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="115" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="116" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="117" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="118" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="119" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="120" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="121" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="122" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="123" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="124" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="125" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="126" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="132" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="133" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="134" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="135" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="136" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="137" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="138" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="139" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="140" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="141" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="142" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="143" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="144" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="145" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="146" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="147" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="148" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="149" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="150" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="151" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="152" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="153" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="154" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="155" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="156" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="157" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="158" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="159" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="160" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="161" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="162" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="163" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="164" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="165" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="166" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="167" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="168" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="169" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="170" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="171" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="172" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="173" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="174" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="175" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="176" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="177" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="178" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="179" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="180" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="181" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="182" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="183" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="184" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="185" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="186" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="187" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="188" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="189" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="190" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="191" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="192" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="193" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="194" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="195" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="196" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="197" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="198" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="199" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="200" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="201" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="202" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="203" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="204" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="205" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="206" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="207" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="208" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="209" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="210" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="211" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="212" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="213" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="214" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="215" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="216" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="217" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="218" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="219" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="220" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="221" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="222" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="223" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="224" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="225" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="226" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="227" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="228" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="229" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="230" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="231" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="232" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="233" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="234" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="235" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="236" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="237" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="238" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="239" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="240" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="241" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="242" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="243" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="244" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="245" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="246" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="247" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="248" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="249" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="250" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="251" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="252" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="253" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="254" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="255" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="256" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="257" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="258" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="259" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="260" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="261" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="262" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="263" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="264" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="265" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="266" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="267" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="268" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="269" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="270" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="271" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="272" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="273" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="274" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="275" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="276" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="277" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="278" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="279" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="280" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="281" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="282" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="283" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="284" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="285" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="286" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="287" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="288" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="289" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="290" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="291" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="292" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="293" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="294" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="295" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="296" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="297" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="298" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="299" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="300" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="301" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="302" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="303" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="304" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="305" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="306" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="307" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="308" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="309" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="310" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="311" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="312" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="313" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="314" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="315" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="316" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="317" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="318" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="319" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="320" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="321" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="322" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="323" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="324" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="325" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="326" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="327" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="328" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="329" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="330" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="331" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="332" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="333" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="334" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="335" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="336" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="337" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="338" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="339" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="340" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="341" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="342" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="343" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="344" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="345" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="346" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="347" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="348" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="349" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="350" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="351" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="352" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="353" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="354" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="355" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="356" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="357" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="358" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="359" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="360" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="361" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="362" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="363" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="364" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="365" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="366" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="367" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="368" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="369" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="370" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="371" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="372" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="373" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="374" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="375" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="376" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="377" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="378" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="379" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="380" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="381" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="382" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="383" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="384" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="385" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="386" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="387" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="388" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="389" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="390" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="391" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="392" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="393" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="394" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="395" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="396" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="397" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="398" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="399" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="400" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="401" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="402" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="403" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="404" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="405" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="406" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="407" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="408" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="409" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="410" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="411" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="412" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="413" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="414" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="415" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="416" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="417" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="418" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="419" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="420" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="421" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="422" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="423" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="424" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="425" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="426" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="427" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="428" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="429" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="430" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="431" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="432" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="433" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="434" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="435" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="436" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="437" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="438" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="439" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="440" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="441" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="442" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="443" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="444" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="445" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="446" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="447" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="448" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="449" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="450" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="451" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="452" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="453" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="454" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="455" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="456" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="457" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="458" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="459" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="460" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="461" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="462" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="463" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="464" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="465" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="466" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="467" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="468" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="469" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="470" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="471" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="472" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="473" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="474" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="475" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="476" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="477" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="478" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="479" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="480" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="481" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="482" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="483" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="484" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="485" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="486" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="487" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="488" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="489" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="490" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="491" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="492" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="493" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="494" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="495" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="496" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="497" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="498" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="499" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="500" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="501" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="502" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="503" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="504" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="505" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="506" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="507" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="508" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="509" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="510" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="511" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="512" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="513" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="514" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="515" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="516" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="517" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="518" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="519" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="520" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="521" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="522" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="523" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="524" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="525" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="526" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="527" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="528" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="529" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="530" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="531" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="532" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="533" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="534" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="535" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="536" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="537" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="538" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="539" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="540" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="541" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="542" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="543" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="544" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="545" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="546" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="547" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="548" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="549" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="550" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="551" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="552" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="553" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="554" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="555" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="556" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="557" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="558" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="559" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="560" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="561" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="562" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="563" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="564" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="565" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="566" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="567" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="568" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="569" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="570" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="571" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="572" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="573" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="574" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="575" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="576" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="577" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="578" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="579" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="580" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="581" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="582" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="583" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="584" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="585" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="586" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="587" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="588" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="589" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="590" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="591" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="592" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="593" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="594" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="595" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="596" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="597" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="598" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="599" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="600" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="601" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="602" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="603" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="604" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="605" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="606" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="607" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="608" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="609" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="610" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="611" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="612" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="613" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="614" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="615" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="616" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="617" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="618" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="619" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="620" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="621" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="622" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="623" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="624" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="625" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="626" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="627" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="628" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="629" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="630" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="631" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="632" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="633" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="634" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="635" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="636" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="637" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="638" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="639" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="640" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="641" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="642" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="643" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="644" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="645" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="646" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="647" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="648" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="649" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="650" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="651" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="652" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="653" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="654" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="655" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="656" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="657" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="658" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="659" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="660" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="661" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="662" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="663" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="664" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="665" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="666" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="667" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="668" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="669" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="670" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="671" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="672" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="673" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="674" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="675" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="676" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="677" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="678" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="679" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="680" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="681" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="682" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="683" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="684" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="685" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="686" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="687" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="688" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="689" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="690" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="691" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="692" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="693" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="694" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="695" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="696" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="697" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="698" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="699" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="700" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="701" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="702" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="703" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="704" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="705" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="706" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="707" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="708" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="709" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="710" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="711" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="712" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="713" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="714" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="715" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="716" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="717" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="718" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="719" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="720" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="721" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="722" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="723" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="724" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="725" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="726" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="727" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="728" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="729" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="730" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="731" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="732" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="733" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="734" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="735" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="736" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="737" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="738" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="739" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="740" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="741" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="742" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="743" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="744" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="745" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="746" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="747" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="748" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="749" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="750" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="751" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="752" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="753" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="754" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="755" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="756" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="757" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="758" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="759" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="760" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="761" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="762" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="763" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="764" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="765" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="766" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="767" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="768" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="769" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="770" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="771" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="772" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="773" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="774" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="775" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="776" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="777" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="778" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="779" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="780" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="781" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="782" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="783" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="784" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="785" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="786" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="787" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="788" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="789" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="790" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="791" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="792" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="793" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="794" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="795" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="796" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="797" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="798" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="799" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="800" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="801" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="802" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="803" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="804" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="805" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="806" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="807" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="808" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="809" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="810" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="811" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="812" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="813" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="814" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="815" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="816" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="817" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="818" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="819" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="820" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="821" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="822" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="823" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="824" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="825" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="826" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="827" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="828" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="829" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="830" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="831" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="832" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="833" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="834" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="835" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="836" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="837" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="838" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="839" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="840" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="841" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="842" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="843" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="844" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="845" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="846" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="847" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="848" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="849" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="850" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="851" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="852" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="853" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="854" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="855" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="856" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="857" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="858" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="859" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="860" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="861" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="862" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="863" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="864" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="865" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="866" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="867" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="868" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="869" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="870" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="871" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="872" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="873" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="874" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="875" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="876" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="877" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="878" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="879" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="880" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="881" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="882" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="883" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="884" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="885" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="886" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="887" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="888" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="889" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="890" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="891" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="892" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="893" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="894" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="895" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="896" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="897" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="898" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="899" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="900" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="901" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="902" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="903" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="904" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="905" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="906" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="907" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="908" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="909" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="910" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="911" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="912" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="913" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="914" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="915" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="916" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="917" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="918" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="919" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="920" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="921" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="922" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="923" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="924" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="925" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="926" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="927" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="928" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="929" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="930" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="931" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="932" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="933" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="934" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="935" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="936" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="937" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="938" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="939" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="940" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="941" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="942" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="943" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="944" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="945" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="946" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="947" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="948" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="949" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="950" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="951" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="J93" s="48"/>
+      <c r="K93" s="49"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
@@ -17253,7 +16768,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="8">
-        <f t="shared" ref="O3:O17" si="1">N3</f>
+        <f t="shared" ref="O3:O5" si="1">N3</f>
         <v>0</v>
       </c>
       <c r="P3" s="40">
@@ -17265,7 +16780,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="8">
-        <f t="shared" ref="S3:S17" si="3">R3</f>
+        <f t="shared" ref="S3:S5" si="3">R3</f>
         <v>0</v>
       </c>
       <c r="T3" s="40">
@@ -17280,7 +16795,7 @@
         <v>2.9</v>
       </c>
       <c r="W3" s="8">
-        <f t="shared" ref="W3:W17" si="5">V3</f>
+        <f t="shared" ref="W3:W5" si="5">V3</f>
         <v>2.9</v>
       </c>
       <c r="X3" s="40">
@@ -17295,7 +16810,7 @@
         <v>14</v>
       </c>
       <c r="AA3" s="8">
-        <f t="shared" ref="AA3:AA17" si="7">Z3</f>
+        <f t="shared" ref="AA3:AA5" si="7">Z3</f>
         <v>14</v>
       </c>
       <c r="AB3" s="40">
@@ -17310,7 +16825,7 @@
         <v>12</v>
       </c>
       <c r="AE3" s="8">
-        <f t="shared" ref="AE3:AE17" si="9">AD3</f>
+        <f t="shared" ref="AE3:AE5" si="9">AD3</f>
         <v>12</v>
       </c>
       <c r="AF3" s="40">
@@ -17765,7 +17280,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="8">
-        <f t="shared" ref="O8:O22" si="11">N8</f>
+        <f t="shared" ref="O8:O10" si="11">N8</f>
         <v>0</v>
       </c>
       <c r="P8" s="40">
@@ -17777,7 +17292,7 @@
         <v>0</v>
       </c>
       <c r="S8" s="8">
-        <f t="shared" ref="S8:S22" si="12">R8</f>
+        <f t="shared" ref="S8:S10" si="12">R8</f>
         <v>0</v>
       </c>
       <c r="T8" s="40">
@@ -17789,7 +17304,7 @@
         <v>0</v>
       </c>
       <c r="W8" s="8">
-        <f t="shared" ref="W8:W22" si="13">V8</f>
+        <f t="shared" ref="W8:W10" si="13">V8</f>
         <v>0</v>
       </c>
       <c r="X8" s="40">
@@ -17804,7 +17319,7 @@
         <v>7.5</v>
       </c>
       <c r="AA8" s="8">
-        <f t="shared" ref="AA8:AA22" si="14">Z8</f>
+        <f t="shared" ref="AA8:AA10" si="14">Z8</f>
         <v>7.5</v>
       </c>
       <c r="AB8" s="40">
@@ -17816,7 +17331,7 @@
         <v>0</v>
       </c>
       <c r="AE8" s="8">
-        <f t="shared" ref="AE8:AE22" si="15">AD8</f>
+        <f t="shared" ref="AE8:AE10" si="15">AD8</f>
         <v>0</v>
       </c>
       <c r="AF8" s="40">
@@ -18235,7 +17750,7 @@
         <v>0</v>
       </c>
       <c r="O13" s="8">
-        <f t="shared" ref="O13:O27" si="16">N13</f>
+        <f t="shared" ref="O13:O15" si="16">N13</f>
         <v>0</v>
       </c>
       <c r="P13" s="40">
@@ -18247,7 +17762,7 @@
         <v>0</v>
       </c>
       <c r="S13" s="8">
-        <f t="shared" ref="S13:S27" si="17">R13</f>
+        <f t="shared" ref="S13:S15" si="17">R13</f>
         <v>0</v>
       </c>
       <c r="T13" s="40">
@@ -18262,7 +17777,7 @@
         <v>0.5</v>
       </c>
       <c r="W13" s="8">
-        <f t="shared" ref="W13:W27" si="18">V13</f>
+        <f t="shared" ref="W13:W15" si="18">V13</f>
         <v>0.5</v>
       </c>
       <c r="X13" s="40">
@@ -18277,7 +17792,7 @@
         <v>1.7</v>
       </c>
       <c r="AA13" s="8">
-        <f t="shared" ref="AA13:AA27" si="19">Z13</f>
+        <f t="shared" ref="AA13:AA15" si="19">Z13</f>
         <v>1.7</v>
       </c>
       <c r="AB13" s="40">
@@ -18292,7 +17807,7 @@
         <v>1</v>
       </c>
       <c r="AE13" s="8">
-        <f t="shared" ref="AE13:AE27" si="20">AD13</f>
+        <f t="shared" ref="AE13:AE15" si="20">AD13</f>
         <v>1</v>
       </c>
       <c r="AF13" s="40">
@@ -19664,7 +19179,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="40">
-        <f t="shared" ref="P27:P29" si="45">O19</f>
+        <f t="shared" ref="P27" si="45">O19</f>
         <v>0</v>
       </c>
       <c r="R27" s="5">
@@ -19676,7 +19191,7 @@
         <v>0</v>
       </c>
       <c r="T27" s="40">
-        <f t="shared" ref="T27:T29" si="46">S19</f>
+        <f t="shared" ref="T27" si="46">S19</f>
         <v>0</v>
       </c>
       <c r="U27" s="4">
@@ -19691,7 +19206,7 @@
         <v>25</v>
       </c>
       <c r="X27" s="40">
-        <f t="shared" ref="X27:X29" si="47">W19</f>
+        <f t="shared" ref="X27" si="47">W19</f>
         <v>25</v>
       </c>
       <c r="Y27" s="4">
@@ -19706,7 +19221,7 @@
         <v>55</v>
       </c>
       <c r="AB27" s="40">
-        <f t="shared" ref="AB27:AB29" si="48">AA19</f>
+        <f t="shared" ref="AB27" si="48">AA19</f>
         <v>50</v>
       </c>
       <c r="AC27" s="4">
@@ -19721,7 +19236,7 @@
         <v>0</v>
       </c>
       <c r="AF27" s="40">
-        <f t="shared" ref="AF27:AF29" si="49">AE19</f>
+        <f t="shared" ref="AF27" si="49">AE19</f>
         <v>78</v>
       </c>
     </row>
@@ -20181,7 +19696,7 @@
         <v>0</v>
       </c>
       <c r="O32" s="8">
-        <f t="shared" ref="O32:O39" si="61">N32</f>
+        <f t="shared" ref="O32:O33" si="61">N32</f>
         <v>0</v>
       </c>
       <c r="P32" s="40">
@@ -20193,7 +19708,7 @@
         <v>0</v>
       </c>
       <c r="S32" s="8">
-        <f t="shared" ref="S32:S39" si="62">R32</f>
+        <f t="shared" ref="S32:S33" si="62">R32</f>
         <v>0</v>
       </c>
       <c r="T32" s="40">
@@ -20208,7 +19723,7 @@
         <v>4</v>
       </c>
       <c r="W32" s="8">
-        <f t="shared" ref="W32:W39" si="63">V32</f>
+        <f t="shared" ref="W32:W33" si="63">V32</f>
         <v>4</v>
       </c>
       <c r="X32" s="40">
@@ -20223,7 +19738,7 @@
         <v>15</v>
       </c>
       <c r="AA32" s="8">
-        <f t="shared" ref="AA32:AA39" si="64">Z32</f>
+        <f t="shared" ref="AA32:AA33" si="64">Z32</f>
         <v>15</v>
       </c>
       <c r="AB32" s="40">
@@ -20235,7 +19750,7 @@
         <v>0</v>
       </c>
       <c r="AE32" s="8">
-        <f t="shared" ref="AE32:AE39" si="65">AD32</f>
+        <f t="shared" ref="AE32:AE33" si="65">AD32</f>
         <v>0</v>
       </c>
       <c r="AF32" s="40">
@@ -20383,75 +19898,75 @@
         <v>5</v>
       </c>
       <c r="N34" s="5">
-        <f t="shared" ref="N34:N58" si="69">$F34*M34</f>
+        <f t="shared" ref="N34:N39" si="69">$F34*M34</f>
         <v>1.25</v>
       </c>
       <c r="O34" s="8">
-        <f t="shared" ref="O34:O37" si="70">$G34*N34</f>
+        <f t="shared" ref="O34" si="70">$G34*N34</f>
         <v>2.5</v>
       </c>
       <c r="P34" s="41">
-        <f t="shared" ref="P34:P55" si="71">$H34*O34</f>
+        <f t="shared" ref="P34" si="71">$H34*O34</f>
         <v>5</v>
       </c>
       <c r="Q34" s="4">
         <v>3</v>
       </c>
       <c r="R34" s="5">
-        <f t="shared" ref="R34:R58" si="72">$F34*Q34</f>
+        <f t="shared" ref="R34:R39" si="72">$F34*Q34</f>
         <v>0.75</v>
       </c>
       <c r="S34" s="8">
-        <f t="shared" ref="S34:S37" si="73">$G34*R34</f>
+        <f t="shared" ref="S34" si="73">$G34*R34</f>
         <v>1.5</v>
       </c>
       <c r="T34" s="41">
-        <f t="shared" ref="T34:T55" si="74">$H34*S34</f>
+        <f t="shared" ref="T34" si="74">$H34*S34</f>
         <v>3</v>
       </c>
       <c r="U34" s="4">
         <v>5</v>
       </c>
       <c r="V34" s="5">
-        <f t="shared" ref="V34:V58" si="75">$F34*U34</f>
+        <f t="shared" ref="V34:V39" si="75">$F34*U34</f>
         <v>1.25</v>
       </c>
       <c r="W34" s="8">
-        <f t="shared" ref="W34:W37" si="76">$G34*V34</f>
+        <f t="shared" ref="W34" si="76">$G34*V34</f>
         <v>2.5</v>
       </c>
       <c r="X34" s="41">
-        <f t="shared" ref="X34:X55" si="77">$H34*W34</f>
+        <f t="shared" ref="X34" si="77">$H34*W34</f>
         <v>5</v>
       </c>
       <c r="Y34" s="4">
         <v>6</v>
       </c>
       <c r="Z34" s="5">
-        <f t="shared" ref="Z34:Z58" si="78">$F34*Y34</f>
+        <f t="shared" ref="Z34:Z39" si="78">$F34*Y34</f>
         <v>1.5</v>
       </c>
       <c r="AA34" s="8">
-        <f t="shared" ref="AA34:AA37" si="79">$G34*Z34</f>
+        <f t="shared" ref="AA34" si="79">$G34*Z34</f>
         <v>3</v>
       </c>
       <c r="AB34" s="41">
-        <f t="shared" ref="AB34:AB55" si="80">$H34*AA34</f>
+        <f t="shared" ref="AB34" si="80">$H34*AA34</f>
         <v>6</v>
       </c>
       <c r="AC34" s="4">
         <v>5</v>
       </c>
       <c r="AD34" s="5">
-        <f t="shared" ref="AD34:AD58" si="81">$F34*AC34</f>
+        <f t="shared" ref="AD34:AD39" si="81">$F34*AC34</f>
         <v>1.25</v>
       </c>
       <c r="AE34" s="8">
-        <f t="shared" ref="AE34:AE37" si="82">$G34*AD34</f>
+        <f t="shared" ref="AE34" si="82">$G34*AD34</f>
         <v>2.5</v>
       </c>
       <c r="AF34" s="41">
-        <f t="shared" ref="AF34:AF55" si="83">$H34*AE34</f>
+        <f t="shared" ref="AF34" si="83">$H34*AE34</f>
         <v>5</v>
       </c>
     </row>
@@ -20739,11 +20254,11 @@
         <v>0.5</v>
       </c>
       <c r="O37" s="8">
-        <f t="shared" ref="O37:O40" si="84">$G37*N37</f>
+        <f t="shared" ref="O37" si="84">$G37*N37</f>
         <v>1</v>
       </c>
       <c r="P37" s="41">
-        <f t="shared" ref="P37:P58" si="85">$H37*O37</f>
+        <f t="shared" ref="P37" si="85">$H37*O37</f>
         <v>2</v>
       </c>
       <c r="R37" s="5">
@@ -20751,11 +20266,11 @@
         <v>0</v>
       </c>
       <c r="S37" s="8">
-        <f t="shared" ref="S37:S40" si="86">$G37*R37</f>
+        <f t="shared" ref="S37" si="86">$G37*R37</f>
         <v>0</v>
       </c>
       <c r="T37" s="41">
-        <f t="shared" ref="T37:T58" si="87">$H37*S37</f>
+        <f t="shared" ref="T37" si="87">$H37*S37</f>
         <v>0</v>
       </c>
       <c r="U37" s="4">
@@ -20766,11 +20281,11 @@
         <v>0.25</v>
       </c>
       <c r="W37" s="8">
-        <f t="shared" ref="W37:W40" si="88">$G37*V37</f>
+        <f t="shared" ref="W37" si="88">$G37*V37</f>
         <v>0.5</v>
       </c>
       <c r="X37" s="41">
-        <f t="shared" ref="X37:X58" si="89">$H37*W37</f>
+        <f t="shared" ref="X37" si="89">$H37*W37</f>
         <v>1</v>
       </c>
       <c r="Z37" s="5">
@@ -20778,11 +20293,11 @@
         <v>0</v>
       </c>
       <c r="AA37" s="8">
-        <f t="shared" ref="AA37:AA40" si="90">$G37*Z37</f>
+        <f t="shared" ref="AA37" si="90">$G37*Z37</f>
         <v>0</v>
       </c>
       <c r="AB37" s="41">
-        <f t="shared" ref="AB37:AB58" si="91">$H37*AA37</f>
+        <f t="shared" ref="AB37" si="91">$H37*AA37</f>
         <v>0</v>
       </c>
       <c r="AD37" s="5">
@@ -20790,11 +20305,11 @@
         <v>0</v>
       </c>
       <c r="AE37" s="8">
-        <f t="shared" ref="AE37:AE40" si="92">$G37*AD37</f>
+        <f t="shared" ref="AE37" si="92">$G37*AD37</f>
         <v>0</v>
       </c>
       <c r="AF37" s="41">
-        <f t="shared" ref="AF37:AF58" si="93">$H37*AE37</f>
+        <f t="shared" ref="AF37" si="93">$H37*AE37</f>
         <v>0</v>
       </c>
     </row>
@@ -21163,7 +20678,7 @@
         <v>0.05</v>
       </c>
       <c r="N41" s="5">
-        <f t="shared" ref="N41:N65" si="100">$F41*M41</f>
+        <f t="shared" ref="N41:N47" si="100">$F41*M41</f>
         <v>0</v>
       </c>
       <c r="O41" s="8">
@@ -21178,7 +20693,7 @@
         <v>1</v>
       </c>
       <c r="R41" s="5">
-        <f t="shared" ref="R41:R65" si="101">$F41*Q41</f>
+        <f t="shared" ref="R41:R47" si="101">$F41*Q41</f>
         <v>0.25</v>
       </c>
       <c r="S41" s="8">
@@ -21193,7 +20708,7 @@
         <v>0.01</v>
       </c>
       <c r="V41" s="5">
-        <f t="shared" ref="V41:V65" si="102">$F41*U41</f>
+        <f t="shared" ref="V41:V47" si="102">$F41*U41</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="W41" s="8">
@@ -21208,7 +20723,7 @@
         <v>0.4</v>
       </c>
       <c r="Z41" s="5">
-        <f t="shared" ref="Z41:Z65" si="103">$F41*Y41</f>
+        <f t="shared" ref="Z41:Z47" si="103">$F41*Y41</f>
         <v>0.1</v>
       </c>
       <c r="AA41" s="8">
@@ -21223,7 +20738,7 @@
         <v>0.1</v>
       </c>
       <c r="AD41" s="5">
-        <f t="shared" ref="AD41:AD65" si="104">$F41*AC41</f>
+        <f t="shared" ref="AD41:AD47" si="104">$F41*AC41</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="AE41" s="8">
@@ -21943,7 +21458,7 @@
         <v>0.3125</v>
       </c>
       <c r="P48" s="41">
-        <f t="shared" ref="P48:P69" si="107">$H48*O48</f>
+        <f t="shared" ref="P48:P55" si="107">$H48*O48</f>
         <v>1</v>
       </c>
       <c r="R48" s="5">
@@ -21955,7 +21470,7 @@
         <v>0</v>
       </c>
       <c r="T48" s="41">
-        <f t="shared" ref="T48:T69" si="109">$H48*S48</f>
+        <f t="shared" ref="T48:T55" si="109">$H48*S48</f>
         <v>0</v>
       </c>
       <c r="U48" s="4">
@@ -21970,7 +21485,7 @@
         <v>0.15625</v>
       </c>
       <c r="X48" s="41">
-        <f t="shared" ref="X48:X69" si="111">$H48*W48</f>
+        <f t="shared" ref="X48:X55" si="111">$H48*W48</f>
         <v>0.5</v>
       </c>
       <c r="Y48" s="4">
@@ -21985,7 +21500,7 @@
         <v>0.3125</v>
       </c>
       <c r="AB48" s="41">
-        <f t="shared" ref="AB48:AB69" si="113">$H48*AA48</f>
+        <f t="shared" ref="AB48:AB55" si="113">$H48*AA48</f>
         <v>1</v>
       </c>
       <c r="AC48" s="4">
@@ -22000,7 +21515,7 @@
         <v>0.15625</v>
       </c>
       <c r="AF48" s="41">
-        <f t="shared" ref="AF48:AF69" si="115">$H48*AE48</f>
+        <f t="shared" ref="AF48:AF55" si="115">$H48*AE48</f>
         <v>0.5</v>
       </c>
     </row>
@@ -22050,7 +21565,7 @@
         <v>50</v>
       </c>
       <c r="N49" s="5">
-        <f t="shared" ref="N49:N73" si="116">$F49*M49</f>
+        <f t="shared" ref="N49:N58" si="116">$F49*M49</f>
         <v>12.5</v>
       </c>
       <c r="O49" s="8">
@@ -22062,7 +21577,7 @@
         <v>50</v>
       </c>
       <c r="R49" s="5">
-        <f t="shared" ref="R49:R73" si="117">$F49*Q49</f>
+        <f t="shared" ref="R49:R58" si="117">$F49*Q49</f>
         <v>0</v>
       </c>
       <c r="S49" s="8">
@@ -22077,7 +21592,7 @@
         <v>30</v>
       </c>
       <c r="V49" s="5">
-        <f t="shared" ref="V49:V73" si="118">$F49*U49</f>
+        <f t="shared" ref="V49:V58" si="118">$F49*U49</f>
         <v>7.5</v>
       </c>
       <c r="W49" s="8">
@@ -22092,7 +21607,7 @@
         <v>40</v>
       </c>
       <c r="Z49" s="5">
-        <f t="shared" ref="Z49:Z73" si="119">$F49*Y49</f>
+        <f t="shared" ref="Z49:Z58" si="119">$F49*Y49</f>
         <v>10</v>
       </c>
       <c r="AA49" s="8">
@@ -22107,7 +21622,7 @@
         <v>15</v>
       </c>
       <c r="AD49" s="5">
-        <f t="shared" ref="AD49:AD73" si="120">$F49*AC49</f>
+        <f t="shared" ref="AD49:AD58" si="120">$F49*AC49</f>
         <v>3.75</v>
       </c>
       <c r="AE49" s="8">
@@ -23261,7 +22776,7 @@
         <v>0</v>
       </c>
       <c r="P60" s="40">
-        <f t="shared" ref="P60:P78" si="127">O60</f>
+        <f t="shared" ref="P60:P77" si="127">O60</f>
         <v>0</v>
       </c>
       <c r="R60" s="5">
@@ -23273,7 +22788,7 @@
         <v>0</v>
       </c>
       <c r="T60" s="40">
-        <f t="shared" ref="T60:T78" si="128">S60</f>
+        <f t="shared" ref="T60:T77" si="128">S60</f>
         <v>0</v>
       </c>
       <c r="U60" s="4">
@@ -23288,7 +22803,7 @@
         <v>2</v>
       </c>
       <c r="X60" s="40">
-        <f t="shared" ref="X60:X78" si="129">W60</f>
+        <f t="shared" ref="X60:X77" si="129">W60</f>
         <v>2</v>
       </c>
       <c r="Z60" s="5">
@@ -23300,7 +22815,7 @@
         <v>0</v>
       </c>
       <c r="AB60" s="40">
-        <f t="shared" ref="AB60:AB78" si="130">AA60</f>
+        <f t="shared" ref="AB60:AB77" si="130">AA60</f>
         <v>0</v>
       </c>
       <c r="AD60" s="5">
@@ -23312,7 +22827,7 @@
         <v>0</v>
       </c>
       <c r="AF60" s="40">
-        <f t="shared" ref="AF60:AF78" si="131">AE60</f>
+        <f t="shared" ref="AF60:AF77" si="131">AE60</f>
         <v>0</v>
       </c>
     </row>
@@ -25097,7 +24612,7 @@
         <v>0</v>
       </c>
       <c r="N79" s="5">
-        <f t="shared" ref="N79:N84" si="148">$F79*M79</f>
+        <f t="shared" ref="N79:N83" si="148">$F79*M79</f>
         <v>0</v>
       </c>
       <c r="O79" s="8">
@@ -25105,11 +24620,11 @@
         <v>0</v>
       </c>
       <c r="P79" s="41">
-        <f t="shared" ref="P79:P84" si="150">$H79*O79</f>
+        <f t="shared" ref="P79" si="150">$H79*O79</f>
         <v>0</v>
       </c>
       <c r="R79" s="5">
-        <f t="shared" ref="R79:R84" si="151">$F79*Q79</f>
+        <f t="shared" ref="R79:R83" si="151">$F79*Q79</f>
         <v>0</v>
       </c>
       <c r="S79" s="8">
@@ -25117,14 +24632,14 @@
         <v>0</v>
       </c>
       <c r="T79" s="41">
-        <f t="shared" ref="T79:T84" si="153">$H79*S79</f>
+        <f t="shared" ref="T79" si="153">$H79*S79</f>
         <v>0</v>
       </c>
       <c r="U79" s="4">
         <v>5</v>
       </c>
       <c r="V79" s="5">
-        <f t="shared" ref="V79:V84" si="154">$F79*U79</f>
+        <f t="shared" ref="V79:V83" si="154">$F79*U79</f>
         <v>1.25</v>
       </c>
       <c r="W79" s="8">
@@ -25132,11 +24647,11 @@
         <v>1.875</v>
       </c>
       <c r="X79" s="41">
-        <f t="shared" ref="X79:X84" si="156">$H79*W79</f>
+        <f t="shared" ref="X79" si="156">$H79*W79</f>
         <v>5</v>
       </c>
       <c r="Z79" s="5">
-        <f t="shared" ref="Z79:Z84" si="157">$F79*Y79</f>
+        <f t="shared" ref="Z79:Z83" si="157">$F79*Y79</f>
         <v>0</v>
       </c>
       <c r="AA79" s="8">
@@ -25144,11 +24659,11 @@
         <v>0</v>
       </c>
       <c r="AB79" s="41">
-        <f t="shared" ref="AB79:AB84" si="159">$H79*AA79</f>
+        <f t="shared" ref="AB79" si="159">$H79*AA79</f>
         <v>0</v>
       </c>
       <c r="AD79" s="5">
-        <f t="shared" ref="AD79:AD84" si="160">$F79*AC79</f>
+        <f t="shared" ref="AD79:AD83" si="160">$F79*AC79</f>
         <v>0</v>
       </c>
       <c r="AE79" s="8">
@@ -25156,7 +24671,7 @@
         <v>0</v>
       </c>
       <c r="AF79" s="41">
-        <f t="shared" ref="AF79:AF84" si="162">$H79*AE79</f>
+        <f t="shared" ref="AF79" si="162">$H79*AE79</f>
         <v>0</v>
       </c>
     </row>
@@ -25332,7 +24847,7 @@
         <v>22.5</v>
       </c>
       <c r="P81" s="41">
-        <f t="shared" ref="P81:P86" si="163">$H81*O81</f>
+        <f t="shared" ref="P81:P83" si="163">$H81*O81</f>
         <v>60</v>
       </c>
       <c r="Q81" s="4">
@@ -25347,7 +24862,7 @@
         <v>1.875</v>
       </c>
       <c r="T81" s="41">
-        <f t="shared" ref="T81:T86" si="164">$H81*S81</f>
+        <f t="shared" ref="T81:T83" si="164">$H81*S81</f>
         <v>5</v>
       </c>
       <c r="U81" s="4">
@@ -25362,7 +24877,7 @@
         <v>5.625</v>
       </c>
       <c r="X81" s="41">
-        <f t="shared" ref="X81:X86" si="165">$H81*W81</f>
+        <f t="shared" ref="X81:X83" si="165">$H81*W81</f>
         <v>15</v>
       </c>
       <c r="Y81" s="4">
@@ -25377,7 +24892,7 @@
         <v>33.75</v>
       </c>
       <c r="AB81" s="41">
-        <f t="shared" ref="AB81:AB86" si="166">$H81*AA81</f>
+        <f t="shared" ref="AB81:AB83" si="166">$H81*AA81</f>
         <v>90</v>
       </c>
       <c r="AC81" s="4">
@@ -25392,7 +24907,7 @@
         <v>26.25</v>
       </c>
       <c r="AF81" s="41">
-        <f t="shared" ref="AF81:AF86" si="167">$H81*AE81</f>
+        <f t="shared" ref="AF81:AF83" si="167">$H81*AE81</f>
         <v>70</v>
       </c>
     </row>
@@ -26584,8 +26099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated mod and high severity fire fine downed wood
</commit_message>
<xml_diff>
--- a/specifications/1_Fire/ScriptRules_Fire.xlsx
+++ b/specifications/1_Fire/ScriptRules_Fire.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\LF\landfiredisturbance\specifications\1_Fire\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HgRepos\LANDFIRE\landfiredisturbance\specifications\1_Fire\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13380" windowHeight="10260" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="FBDescriptions" sheetId="9" r:id="rId1"/>
@@ -1216,9 +1216,6 @@
     <t>* = 1 /(0.5*1.25)</t>
   </si>
   <si>
-    <t>* = 1/(0.25*1.25)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> + = OTree_Density * 0.4 + MidTree_Density * 0.4</t>
   </si>
   <si>
@@ -1315,9 +1312,6 @@
     <t>* = 1/0.05</t>
   </si>
   <si>
-    <t>* = 1/(0.05*1.5)</t>
-  </si>
-  <si>
     <t>* = (1/0.05)</t>
   </si>
   <si>
@@ -1343,6 +1337,12 @@
   </si>
   <si>
     <t>* = (1/0.05)*0.5</t>
+  </si>
+  <si>
+    <t>* = (1/(0.25*1.25))*0.33</t>
+  </si>
+  <si>
+    <t>* = (1/(0.05*1.5))*0.33</t>
   </si>
 </sst>
 </file>
@@ -2541,8 +2541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K93"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2960,24 +2960,24 @@
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="14" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H18" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I18" s="13"/>
       <c r="J18" s="14" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -2989,24 +2989,24 @@
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="F19" s="13"/>
       <c r="G19" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I19" s="13"/>
       <c r="J19" s="14" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="K19" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3018,24 +3018,24 @@
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>405</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>406</v>
       </c>
       <c r="F20" s="13"/>
       <c r="G20" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="H20" s="15" t="s">
         <v>405</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>406</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="14" t="s">
+        <v>404</v>
+      </c>
+      <c r="K20" s="15" t="s">
         <v>405</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3046,29 +3046,29 @@
         <v>297</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D21" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E21" s="18"/>
       <c r="F21" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="G21" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I21" s="13" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J21" s="21" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3079,29 +3079,29 @@
         <v>298</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E22" s="18"/>
       <c r="F22" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J22" s="21" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3112,29 +3112,29 @@
         <v>299</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D23" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E23" s="18"/>
       <c r="F23" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H23" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3145,29 +3145,29 @@
         <v>300</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D24" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E24" s="18"/>
       <c r="F24" s="13" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G24" s="21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="J24" s="21" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3178,29 +3178,29 @@
         <v>301</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E25" s="18"/>
       <c r="F25" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="G25" s="21" t="s">
         <v>413</v>
       </c>
-      <c r="G25" s="21" t="s">
-        <v>414</v>
-      </c>
       <c r="H25" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I25" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="J25" s="14" t="s">
         <v>416</v>
       </c>
-      <c r="J25" s="14" t="s">
-        <v>417</v>
-      </c>
       <c r="K25" s="15" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3212,24 +3212,24 @@
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="F26" s="13"/>
       <c r="G26" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="14" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="K26" s="20" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3241,24 +3241,24 @@
       </c>
       <c r="C27" s="13"/>
       <c r="D27" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F27" s="13"/>
       <c r="G27" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="14" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="K27" s="20" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3270,24 +3270,24 @@
       </c>
       <c r="C28" s="13"/>
       <c r="D28" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="F28" s="13"/>
       <c r="G28" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I28" s="13"/>
       <c r="J28" s="14" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="K28" s="20" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3299,24 +3299,24 @@
       </c>
       <c r="C29" s="13"/>
       <c r="D29" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F29" s="13"/>
       <c r="G29" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I29" s="13"/>
       <c r="J29" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K29" s="20" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3328,24 +3328,24 @@
       </c>
       <c r="C30" s="13"/>
       <c r="D30" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F30" s="13"/>
       <c r="G30" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="14" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3357,24 +3357,24 @@
       </c>
       <c r="C31" s="13"/>
       <c r="D31" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="F31" s="13"/>
       <c r="G31" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3431,7 +3431,7 @@
         <v>5</v>
       </c>
       <c r="G34" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H34" s="15" t="s">
         <v>391</v>
@@ -3466,10 +3466,10 @@
         <v>5</v>
       </c>
       <c r="G35" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I35" s="13" t="s">
         <v>21</v>
@@ -3478,7 +3478,7 @@
         <v>23</v>
       </c>
       <c r="K35" s="15" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3508,7 +3508,7 @@
         <v>21</v>
       </c>
       <c r="J36" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K36" s="15"/>
     </row>
@@ -3532,7 +3532,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H37" s="15" t="s">
         <v>391</v>
@@ -3567,10 +3567,10 @@
         <v>5</v>
       </c>
       <c r="G38" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H38" s="15" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="I38" s="13" t="s">
         <v>21</v>
@@ -3579,7 +3579,7 @@
         <v>23</v>
       </c>
       <c r="K38" s="15" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3609,7 +3609,7 @@
         <v>21</v>
       </c>
       <c r="J39" s="14" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="K39" s="15"/>
     </row>
@@ -3638,7 +3638,7 @@
         <v>21</v>
       </c>
       <c r="J40" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K40" s="15"/>
     </row>
@@ -3660,14 +3660,14 @@
         <v>5</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H41" s="15"/>
       <c r="I41" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J41" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K41" s="15"/>
     </row>
@@ -3689,14 +3689,14 @@
         <v>5</v>
       </c>
       <c r="G42" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H42" s="15"/>
       <c r="I42" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J42" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K42" s="15"/>
     </row>
@@ -3725,7 +3725,7 @@
         <v>21</v>
       </c>
       <c r="J43" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K43" s="15"/>
     </row>
@@ -3754,7 +3754,7 @@
         <v>21</v>
       </c>
       <c r="J44" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K44" s="15"/>
     </row>
@@ -3776,14 +3776,14 @@
         <v>5</v>
       </c>
       <c r="G45" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H45" s="15"/>
       <c r="I45" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J45" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K45" s="15"/>
     </row>
@@ -3805,14 +3805,14 @@
         <v>5</v>
       </c>
       <c r="G46" s="14" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H46" s="15"/>
       <c r="I46" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J46" s="14" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="K46" s="15"/>
     </row>
@@ -3841,7 +3841,7 @@
         <v>21</v>
       </c>
       <c r="J47" s="14" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K47" s="15"/>
     </row>
@@ -3868,7 +3868,7 @@
         <v>14</v>
       </c>
       <c r="H48" s="15" t="s">
-        <v>394</v>
+        <v>435</v>
       </c>
       <c r="I48" s="13" t="s">
         <v>21</v>
@@ -3877,7 +3877,7 @@
         <v>18</v>
       </c>
       <c r="K48" s="15" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="49" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3903,7 +3903,7 @@
         <v>14</v>
       </c>
       <c r="H49" s="15" t="s">
-        <v>394</v>
+        <v>435</v>
       </c>
       <c r="I49" s="13" t="s">
         <v>21</v>
@@ -3912,7 +3912,7 @@
         <v>18</v>
       </c>
       <c r="K49" s="15" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="50" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3938,7 +3938,7 @@
         <v>14</v>
       </c>
       <c r="H50" s="15" t="s">
-        <v>394</v>
+        <v>435</v>
       </c>
       <c r="I50" s="13" t="s">
         <v>21</v>
@@ -3947,7 +3947,7 @@
         <v>18</v>
       </c>
       <c r="K50" s="15" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="51" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -3973,7 +3973,7 @@
         <v>14</v>
       </c>
       <c r="H51" s="15" t="s">
-        <v>394</v>
+        <v>435</v>
       </c>
       <c r="I51" s="13" t="s">
         <v>21</v>
@@ -3982,7 +3982,7 @@
         <v>18</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="52" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4008,7 +4008,7 @@
         <v>14</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>394</v>
+        <v>435</v>
       </c>
       <c r="I52" s="13" t="s">
         <v>21</v>
@@ -4017,7 +4017,7 @@
         <v>18</v>
       </c>
       <c r="K52" s="15" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
     </row>
     <row r="53" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4136,28 +4136,28 @@
         <v>0</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F56" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G56" s="22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H56" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I56" s="13" t="s">
         <v>3</v>
       </c>
       <c r="J56" s="22" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K56" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="57" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4171,28 +4171,28 @@
         <v>0</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E57" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F57" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G57" s="22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="I57" s="13" t="s">
         <v>3</v>
       </c>
       <c r="J57" s="22" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="58" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4206,28 +4206,28 @@
         <v>0</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E58" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F58" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G58" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I58" s="13" t="s">
         <v>3</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4625,19 +4625,19 @@
         <v>5</v>
       </c>
       <c r="G78" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H78" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I78" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J78" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K78" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="79" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4658,19 +4658,19 @@
         <v>5</v>
       </c>
       <c r="G79" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H79" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I79" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J79" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K79" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="80" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4691,19 +4691,19 @@
         <v>5</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H80" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I80" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J80" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K80" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="81" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4724,19 +4724,19 @@
         <v>5</v>
       </c>
       <c r="G81" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H81" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I81" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J81" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K81" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="82" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4757,19 +4757,19 @@
         <v>5</v>
       </c>
       <c r="G82" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H82" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I82" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J82" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K82" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="83" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -4790,19 +4790,19 @@
         <v>5</v>
       </c>
       <c r="G83" s="14" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H83" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I83" s="13" t="s">
         <v>21</v>
       </c>
       <c r="J83" s="14" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="K83" s="15" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="84" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -16495,10 +16495,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <pane ySplit="450" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1:N1048576"/>
-      <selection pane="bottomLeft" activeCell="AB2" sqref="AB2"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16755,7 +16755,7 @@
         <v>0</v>
       </c>
       <c r="L3" s="8">
-        <f t="shared" ref="L3:L17" si="1">K3</f>
+        <f t="shared" ref="L3:L5" si="1">K3</f>
         <v>0</v>
       </c>
       <c r="M3" s="40">
@@ -16767,7 +16767,7 @@
         <v>0</v>
       </c>
       <c r="P3" s="8">
-        <f t="shared" ref="P3:P17" si="3">O3</f>
+        <f t="shared" ref="P3:P5" si="3">O3</f>
         <v>0</v>
       </c>
       <c r="Q3" s="40">
@@ -16782,7 +16782,7 @@
         <v>2.9</v>
       </c>
       <c r="T3" s="8">
-        <f t="shared" ref="T3:T17" si="5">S3</f>
+        <f t="shared" ref="T3:T5" si="5">S3</f>
         <v>2.9</v>
       </c>
       <c r="U3" s="40">
@@ -16797,7 +16797,7 @@
         <v>14</v>
       </c>
       <c r="X3" s="8">
-        <f t="shared" ref="X3:X17" si="7">W3</f>
+        <f t="shared" ref="X3:X5" si="7">W3</f>
         <v>14</v>
       </c>
       <c r="Y3" s="40">
@@ -16812,7 +16812,7 @@
         <v>12</v>
       </c>
       <c r="AB3" s="8">
-        <f t="shared" ref="AB3:AB17" si="9">AA3</f>
+        <f t="shared" ref="AB3:AB5" si="9">AA3</f>
         <v>12</v>
       </c>
       <c r="AC3" s="40">
@@ -17242,7 +17242,7 @@
         <v>0</v>
       </c>
       <c r="L8" s="8">
-        <f t="shared" ref="L8:L22" si="11">K8</f>
+        <f t="shared" ref="L8:L10" si="11">K8</f>
         <v>0</v>
       </c>
       <c r="M8" s="40">
@@ -17254,7 +17254,7 @@
         <v>0</v>
       </c>
       <c r="P8" s="8">
-        <f t="shared" ref="P8:P22" si="12">O8</f>
+        <f t="shared" ref="P8:P10" si="12">O8</f>
         <v>0</v>
       </c>
       <c r="Q8" s="40">
@@ -17266,7 +17266,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="8">
-        <f t="shared" ref="T8:T22" si="13">S8</f>
+        <f t="shared" ref="T8:T10" si="13">S8</f>
         <v>0</v>
       </c>
       <c r="U8" s="40">
@@ -17281,7 +17281,7 @@
         <v>7.5</v>
       </c>
       <c r="X8" s="8">
-        <f t="shared" ref="X8:X22" si="14">W8</f>
+        <f t="shared" ref="X8:X10" si="14">W8</f>
         <v>7.5</v>
       </c>
       <c r="Y8" s="40">
@@ -17293,7 +17293,7 @@
         <v>0</v>
       </c>
       <c r="AB8" s="8">
-        <f t="shared" ref="AB8:AB22" si="15">AA8</f>
+        <f t="shared" ref="AB8:AB10" si="15">AA8</f>
         <v>0</v>
       </c>
       <c r="AC8" s="40">
@@ -17687,7 +17687,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="8">
-        <f t="shared" ref="L13:L27" si="16">K13</f>
+        <f t="shared" ref="L13:L15" si="16">K13</f>
         <v>0</v>
       </c>
       <c r="M13" s="40">
@@ -17699,7 +17699,7 @@
         <v>0</v>
       </c>
       <c r="P13" s="8">
-        <f t="shared" ref="P13:P27" si="17">O13</f>
+        <f t="shared" ref="P13:P15" si="17">O13</f>
         <v>0</v>
       </c>
       <c r="Q13" s="40">
@@ -17714,7 +17714,7 @@
         <v>0.5</v>
       </c>
       <c r="T13" s="8">
-        <f t="shared" ref="T13:T27" si="18">S13</f>
+        <f t="shared" ref="T13:T15" si="18">S13</f>
         <v>0.5</v>
       </c>
       <c r="U13" s="40">
@@ -17729,7 +17729,7 @@
         <v>1.7</v>
       </c>
       <c r="X13" s="8">
-        <f t="shared" ref="X13:X27" si="19">W13</f>
+        <f t="shared" ref="X13:X15" si="19">W13</f>
         <v>1.7</v>
       </c>
       <c r="Y13" s="40">
@@ -17744,7 +17744,7 @@
         <v>1</v>
       </c>
       <c r="AB13" s="8">
-        <f t="shared" ref="AB13:AB27" si="20">AA13</f>
+        <f t="shared" ref="AB13:AB15" si="20">AA13</f>
         <v>1</v>
       </c>
       <c r="AC13" s="40">
@@ -18797,7 +18797,7 @@
         <v>301</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D25" s="37" t="s">
         <v>379</v>
@@ -19014,7 +19014,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="40">
-        <f t="shared" ref="M27:M29" si="45">L19</f>
+        <f t="shared" ref="M27" si="45">L19</f>
         <v>0</v>
       </c>
       <c r="O27" s="5">
@@ -19026,7 +19026,7 @@
         <v>0</v>
       </c>
       <c r="Q27" s="40">
-        <f t="shared" ref="Q27:Q29" si="46">P19</f>
+        <f t="shared" ref="Q27" si="46">P19</f>
         <v>0</v>
       </c>
       <c r="R27" s="4">
@@ -19041,7 +19041,7 @@
         <v>25</v>
       </c>
       <c r="U27" s="40">
-        <f t="shared" ref="U27:U29" si="47">T19</f>
+        <f t="shared" ref="U27" si="47">T19</f>
         <v>25</v>
       </c>
       <c r="V27" s="4">
@@ -19056,7 +19056,7 @@
         <v>55</v>
       </c>
       <c r="Y27" s="40">
-        <f t="shared" ref="Y27:Y29" si="48">X19</f>
+        <f t="shared" ref="Y27" si="48">X19</f>
         <v>50</v>
       </c>
       <c r="Z27" s="4">
@@ -19071,7 +19071,7 @@
         <v>0</v>
       </c>
       <c r="AC27" s="40">
-        <f t="shared" ref="AC27:AC29" si="49">AB19</f>
+        <f t="shared" ref="AC27" si="49">AB19</f>
         <v>78</v>
       </c>
     </row>
@@ -19500,7 +19500,7 @@
         <v>0</v>
       </c>
       <c r="L32" s="8">
-        <f t="shared" ref="L32:L39" si="61">K32</f>
+        <f t="shared" ref="L32:L33" si="61">K32</f>
         <v>0</v>
       </c>
       <c r="M32" s="40">
@@ -19512,7 +19512,7 @@
         <v>0</v>
       </c>
       <c r="P32" s="8">
-        <f t="shared" ref="P32:P39" si="62">O32</f>
+        <f t="shared" ref="P32:P33" si="62">O32</f>
         <v>0</v>
       </c>
       <c r="Q32" s="40">
@@ -19527,7 +19527,7 @@
         <v>4</v>
       </c>
       <c r="T32" s="8">
-        <f t="shared" ref="T32:T39" si="63">S32</f>
+        <f t="shared" ref="T32:T33" si="63">S32</f>
         <v>4</v>
       </c>
       <c r="U32" s="40">
@@ -19542,7 +19542,7 @@
         <v>15</v>
       </c>
       <c r="X32" s="8">
-        <f t="shared" ref="X32:X39" si="64">W32</f>
+        <f t="shared" ref="X32:X33" si="64">W32</f>
         <v>15</v>
       </c>
       <c r="Y32" s="40">
@@ -19554,7 +19554,7 @@
         <v>0</v>
       </c>
       <c r="AB32" s="8">
-        <f t="shared" ref="AB32:AB39" si="65">AA32</f>
+        <f t="shared" ref="AB32:AB33" si="65">AA32</f>
         <v>0</v>
       </c>
       <c r="AC32" s="40">
@@ -19690,11 +19690,11 @@
         <v>5</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" ref="K34:K58" si="68">$C34*J34</f>
+        <f t="shared" ref="K34:K39" si="68">$C34*J34</f>
         <v>1.25</v>
       </c>
       <c r="L34" s="8">
-        <f t="shared" ref="L34:L37" si="69">$D34*K34</f>
+        <f t="shared" ref="L34" si="69">$D34*K34</f>
         <v>2.5</v>
       </c>
       <c r="M34" s="41">
@@ -19705,11 +19705,11 @@
         <v>3</v>
       </c>
       <c r="O34" s="5">
-        <f t="shared" ref="O34:O58" si="70">$C34*N34</f>
+        <f t="shared" ref="O34:O39" si="70">$C34*N34</f>
         <v>0.75</v>
       </c>
       <c r="P34" s="8">
-        <f t="shared" ref="P34:P37" si="71">$D34*O34</f>
+        <f t="shared" ref="P34" si="71">$D34*O34</f>
         <v>1.5</v>
       </c>
       <c r="Q34" s="41">
@@ -19720,11 +19720,11 @@
         <v>5</v>
       </c>
       <c r="S34" s="5">
-        <f t="shared" ref="S34:S58" si="72">$C34*R34</f>
+        <f t="shared" ref="S34:S39" si="72">$C34*R34</f>
         <v>1.25</v>
       </c>
       <c r="T34" s="8">
-        <f t="shared" ref="T34:T37" si="73">$D34*S34</f>
+        <f t="shared" ref="T34" si="73">$D34*S34</f>
         <v>2.5</v>
       </c>
       <c r="U34" s="41">
@@ -19735,11 +19735,11 @@
         <v>6</v>
       </c>
       <c r="W34" s="5">
-        <f t="shared" ref="W34:W58" si="74">$C34*V34</f>
+        <f t="shared" ref="W34:W39" si="74">$C34*V34</f>
         <v>1.5</v>
       </c>
       <c r="X34" s="8">
-        <f t="shared" ref="X34:X37" si="75">$D34*W34</f>
+        <f t="shared" ref="X34" si="75">$D34*W34</f>
         <v>3</v>
       </c>
       <c r="Y34" s="41">
@@ -19750,11 +19750,11 @@
         <v>5</v>
       </c>
       <c r="AA34" s="5">
-        <f t="shared" ref="AA34:AA58" si="76">$C34*Z34</f>
+        <f t="shared" ref="AA34:AA39" si="76">$C34*Z34</f>
         <v>1.25</v>
       </c>
       <c r="AB34" s="8">
-        <f t="shared" ref="AB34:AB37" si="77">$D34*AA34</f>
+        <f t="shared" ref="AB34" si="77">$D34*AA34</f>
         <v>2.5</v>
       </c>
       <c r="AC34" s="41">
@@ -20021,7 +20021,7 @@
         <v>0.5</v>
       </c>
       <c r="L37" s="8">
-        <f t="shared" ref="L37:L40" si="78">$D37*K37</f>
+        <f t="shared" ref="L37" si="78">$D37*K37</f>
         <v>1</v>
       </c>
       <c r="M37" s="41">
@@ -20033,7 +20033,7 @@
         <v>0</v>
       </c>
       <c r="P37" s="8">
-        <f t="shared" ref="P37:P40" si="79">$D37*O37</f>
+        <f t="shared" ref="P37" si="79">$D37*O37</f>
         <v>0</v>
       </c>
       <c r="Q37" s="41">
@@ -20048,7 +20048,7 @@
         <v>0.25</v>
       </c>
       <c r="T37" s="8">
-        <f t="shared" ref="T37:T40" si="80">$D37*S37</f>
+        <f t="shared" ref="T37" si="80">$D37*S37</f>
         <v>0.5</v>
       </c>
       <c r="U37" s="41">
@@ -20060,7 +20060,7 @@
         <v>0</v>
       </c>
       <c r="X37" s="8">
-        <f t="shared" ref="X37:X40" si="81">$D37*W37</f>
+        <f t="shared" ref="X37" si="81">$D37*W37</f>
         <v>0</v>
       </c>
       <c r="Y37" s="41">
@@ -20072,7 +20072,7 @@
         <v>0</v>
       </c>
       <c r="AB37" s="8">
-        <f t="shared" ref="AB37:AB40" si="82">$D37*AA37</f>
+        <f t="shared" ref="AB37" si="82">$D37*AA37</f>
         <v>0</v>
       </c>
       <c r="AC37" s="41">
@@ -20415,7 +20415,7 @@
         <v>0.15000000000000002</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" ref="K41:K65" si="89">$C41*J41</f>
+        <f t="shared" ref="K41:K47" si="89">$C41*J41</f>
         <v>0</v>
       </c>
       <c r="L41" s="8">
@@ -20430,7 +20430,7 @@
         <v>1</v>
       </c>
       <c r="O41" s="5">
-        <f t="shared" ref="O41:O65" si="90">$C41*N41</f>
+        <f t="shared" ref="O41:O47" si="90">$C41*N41</f>
         <v>0.25</v>
       </c>
       <c r="P41" s="8">
@@ -20445,7 +20445,7 @@
         <v>0.01</v>
       </c>
       <c r="S41" s="5">
-        <f t="shared" ref="S41:S65" si="91">$C41*R41</f>
+        <f t="shared" ref="S41:S47" si="91">$C41*R41</f>
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="T41" s="8">
@@ -20460,7 +20460,7 @@
         <v>0.4</v>
       </c>
       <c r="W41" s="5">
-        <f t="shared" ref="W41:W65" si="92">$C41*V41</f>
+        <f t="shared" ref="W41:W47" si="92">$C41*V41</f>
         <v>0.1</v>
       </c>
       <c r="X41" s="8">
@@ -20475,7 +20475,7 @@
         <v>0.1</v>
       </c>
       <c r="AA41" s="5">
-        <f t="shared" ref="AA41:AA65" si="93">$C41*Z41</f>
+        <f t="shared" ref="AA41:AA47" si="93">$C41*Z41</f>
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="AB41" s="8">
@@ -21114,8 +21114,8 @@
         <v>1.25</v>
       </c>
       <c r="E48" s="31">
-        <f>1/(0.25*1.25)</f>
-        <v>3.2</v>
+        <f>1/(0.25*1.25)*0.33</f>
+        <v>1.056</v>
       </c>
       <c r="F48" s="4">
         <v>4</v>
@@ -21130,7 +21130,7 @@
       </c>
       <c r="I48" s="41">
         <f t="shared" ref="I48:I55" si="95">$E48*H48</f>
-        <v>4</v>
+        <v>1.32</v>
       </c>
       <c r="J48" s="4">
         <v>1</v>
@@ -21145,7 +21145,7 @@
       </c>
       <c r="M48" s="41">
         <f t="shared" ref="M48:M55" si="97">$E48*L48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="O48" s="5">
         <f>$C48*N48</f>
@@ -21172,7 +21172,7 @@
       </c>
       <c r="U48" s="41">
         <f t="shared" ref="U48:U55" si="101">$E48*T48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="V48" s="4">
         <v>1</v>
@@ -21187,7 +21187,7 @@
       </c>
       <c r="Y48" s="41">
         <f t="shared" ref="Y48:Y55" si="103">$E48*X48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="Z48" s="4">
         <v>0.5</v>
@@ -21202,7 +21202,7 @@
       </c>
       <c r="AC48" s="41">
         <f t="shared" ref="AC48:AC55" si="105">$E48*AB48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -21220,8 +21220,8 @@
         <v>1.25</v>
       </c>
       <c r="E49" s="31">
-        <f>1/(0.25*1.25)</f>
-        <v>3.2</v>
+        <f>1/(0.25*1.25)*0.33</f>
+        <v>1.056</v>
       </c>
       <c r="F49" s="4">
         <v>70</v>
@@ -21236,13 +21236,13 @@
       </c>
       <c r="I49" s="41">
         <f t="shared" si="95"/>
-        <v>70</v>
+        <v>23.1</v>
       </c>
       <c r="J49" s="4">
         <v>50</v>
       </c>
       <c r="K49" s="5">
-        <f t="shared" ref="K49:K73" si="106">$C49*J49</f>
+        <f t="shared" ref="K49:K58" si="106">$C49*J49</f>
         <v>12.5</v>
       </c>
       <c r="L49" s="8">
@@ -21251,10 +21251,10 @@
       </c>
       <c r="M49" s="41">
         <f t="shared" si="97"/>
-        <v>50</v>
+        <v>16.5</v>
       </c>
       <c r="O49" s="5">
-        <f t="shared" ref="O49:O73" si="107">$C49*N49</f>
+        <f t="shared" ref="O49:O58" si="107">$C49*N49</f>
         <v>0</v>
       </c>
       <c r="P49" s="8">
@@ -21269,7 +21269,7 @@
         <v>30</v>
       </c>
       <c r="S49" s="5">
-        <f t="shared" ref="S49:S73" si="108">$C49*R49</f>
+        <f t="shared" ref="S49:S58" si="108">$C49*R49</f>
         <v>7.5</v>
       </c>
       <c r="T49" s="8">
@@ -21278,13 +21278,13 @@
       </c>
       <c r="U49" s="41">
         <f t="shared" si="101"/>
-        <v>30</v>
+        <v>9.9</v>
       </c>
       <c r="V49" s="4">
         <v>40</v>
       </c>
       <c r="W49" s="5">
-        <f t="shared" ref="W49:W73" si="109">$C49*V49</f>
+        <f t="shared" ref="W49:W58" si="109">$C49*V49</f>
         <v>10</v>
       </c>
       <c r="X49" s="8">
@@ -21293,13 +21293,13 @@
       </c>
       <c r="Y49" s="41">
         <f t="shared" si="103"/>
-        <v>40</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="Z49" s="4">
         <v>15</v>
       </c>
       <c r="AA49" s="5">
-        <f t="shared" ref="AA49:AA73" si="110">$C49*Z49</f>
+        <f t="shared" ref="AA49:AA58" si="110">$C49*Z49</f>
         <v>3.75</v>
       </c>
       <c r="AB49" s="8">
@@ -21308,7 +21308,7 @@
       </c>
       <c r="AC49" s="41">
         <f t="shared" si="105"/>
-        <v>15</v>
+        <v>4.95</v>
       </c>
     </row>
     <row r="50" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -21326,8 +21326,8 @@
         <v>1.25</v>
       </c>
       <c r="E50" s="31">
-        <f>1/(0.25*1.25)</f>
-        <v>3.2</v>
+        <f>1/(0.25*1.25)*0.33</f>
+        <v>1.056</v>
       </c>
       <c r="F50" s="4">
         <v>2</v>
@@ -21342,7 +21342,7 @@
       </c>
       <c r="I50" s="41">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>0.66</v>
       </c>
       <c r="J50" s="4">
         <v>1</v>
@@ -21357,7 +21357,7 @@
       </c>
       <c r="M50" s="41">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="O50" s="5">
         <f t="shared" si="107"/>
@@ -21384,7 +21384,7 @@
       </c>
       <c r="U50" s="41">
         <f t="shared" si="101"/>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="V50" s="4">
         <v>1</v>
@@ -21399,7 +21399,7 @@
       </c>
       <c r="Y50" s="41">
         <f t="shared" si="103"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="Z50" s="4">
         <v>0.3</v>
@@ -21414,7 +21414,7 @@
       </c>
       <c r="AC50" s="41">
         <f t="shared" si="105"/>
-        <v>0.30000000000000004</v>
+        <v>9.9000000000000005E-2</v>
       </c>
     </row>
     <row r="51" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -21432,8 +21432,8 @@
         <v>1.25</v>
       </c>
       <c r="E51" s="31">
-        <f>1/(0.25*1.25)</f>
-        <v>3.2</v>
+        <f>1/(0.25*1.25)*0.33</f>
+        <v>1.056</v>
       </c>
       <c r="F51" s="4">
         <v>1.5</v>
@@ -21448,7 +21448,7 @@
       </c>
       <c r="I51" s="41">
         <f t="shared" si="95"/>
-        <v>1.5</v>
+        <v>0.495</v>
       </c>
       <c r="J51" s="4">
         <v>1</v>
@@ -21463,7 +21463,7 @@
       </c>
       <c r="M51" s="41">
         <f t="shared" si="97"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="O51" s="5">
         <f t="shared" si="107"/>
@@ -21490,7 +21490,7 @@
       </c>
       <c r="U51" s="41">
         <f t="shared" si="101"/>
-        <v>0.2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="V51" s="4">
         <v>0.5</v>
@@ -21505,7 +21505,7 @@
       </c>
       <c r="Y51" s="41">
         <f t="shared" si="103"/>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="Z51" s="4">
         <v>0.4</v>
@@ -21520,7 +21520,7 @@
       </c>
       <c r="AC51" s="41">
         <f t="shared" si="105"/>
-        <v>0.4</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -21538,8 +21538,8 @@
         <v>1.25</v>
       </c>
       <c r="E52" s="31">
-        <f>1/(0.25*1.25)</f>
-        <v>3.2</v>
+        <f>1/(0.25*1.25)*0.33</f>
+        <v>1.056</v>
       </c>
       <c r="F52" s="4">
         <v>1</v>
@@ -21554,7 +21554,7 @@
       </c>
       <c r="I52" s="41">
         <f t="shared" si="95"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="J52" s="4">
         <v>0.5</v>
@@ -21569,7 +21569,7 @@
       </c>
       <c r="M52" s="41">
         <f t="shared" si="97"/>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="O52" s="5">
         <f t="shared" si="107"/>
@@ -21596,7 +21596,7 @@
       </c>
       <c r="U52" s="41">
         <f t="shared" si="101"/>
-        <v>0.1</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="V52" s="4">
         <v>0.3</v>
@@ -21611,7 +21611,7 @@
       </c>
       <c r="Y52" s="41">
         <f t="shared" si="103"/>
-        <v>0.30000000000000004</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="Z52" s="4">
         <v>0.02</v>
@@ -21626,7 +21626,7 @@
       </c>
       <c r="AC52" s="41">
         <f t="shared" si="105"/>
-        <v>2.0000000000000004E-2</v>
+        <v>6.6000000000000008E-3</v>
       </c>
     </row>
     <row r="53" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -22366,7 +22366,7 @@
         <v>0</v>
       </c>
       <c r="M60" s="40">
-        <f t="shared" ref="M60:M78" si="117">L60</f>
+        <f t="shared" ref="M60:M77" si="117">L60</f>
         <v>0</v>
       </c>
       <c r="O60" s="5">
@@ -22378,7 +22378,7 @@
         <v>0</v>
       </c>
       <c r="Q60" s="40">
-        <f t="shared" ref="Q60:Q78" si="118">P60</f>
+        <f t="shared" ref="Q60:Q77" si="118">P60</f>
         <v>0</v>
       </c>
       <c r="R60" s="4">
@@ -22393,7 +22393,7 @@
         <v>2</v>
       </c>
       <c r="U60" s="40">
-        <f t="shared" ref="U60:U78" si="119">T60</f>
+        <f t="shared" ref="U60:U77" si="119">T60</f>
         <v>2</v>
       </c>
       <c r="W60" s="5">
@@ -22405,7 +22405,7 @@
         <v>0</v>
       </c>
       <c r="Y60" s="40">
-        <f t="shared" ref="Y60:Y78" si="120">X60</f>
+        <f t="shared" ref="Y60:Y77" si="120">X60</f>
         <v>0</v>
       </c>
       <c r="AA60" s="5">
@@ -22417,7 +22417,7 @@
         <v>0</v>
       </c>
       <c r="AC60" s="40">
-        <f t="shared" ref="AC60:AC78" si="121">AB60</f>
+        <f t="shared" ref="AC60:AC77" si="121">AB60</f>
         <v>0</v>
       </c>
     </row>
@@ -24123,7 +24123,7 @@
         <v>0</v>
       </c>
       <c r="M79" s="41">
-        <f t="shared" ref="M79:M83" si="140">$E79*L79</f>
+        <f t="shared" ref="M79" si="140">$E79*L79</f>
         <v>0</v>
       </c>
       <c r="O79" s="5">
@@ -24135,7 +24135,7 @@
         <v>0</v>
       </c>
       <c r="Q79" s="41">
-        <f t="shared" ref="Q79:Q83" si="143">$E79*P79</f>
+        <f t="shared" ref="Q79" si="143">$E79*P79</f>
         <v>0</v>
       </c>
       <c r="R79" s="4">
@@ -24150,7 +24150,7 @@
         <v>2.5</v>
       </c>
       <c r="U79" s="41">
-        <f t="shared" ref="U79:U83" si="146">$E79*T79</f>
+        <f t="shared" ref="U79" si="146">$E79*T79</f>
         <v>5</v>
       </c>
       <c r="W79" s="5">
@@ -24162,7 +24162,7 @@
         <v>0</v>
       </c>
       <c r="Y79" s="41">
-        <f t="shared" ref="Y79:Y83" si="149">$E79*X79</f>
+        <f t="shared" ref="Y79" si="149">$E79*X79</f>
         <v>0</v>
       </c>
       <c r="AA79" s="5">
@@ -24174,7 +24174,7 @@
         <v>0</v>
       </c>
       <c r="AC79" s="41">
-        <f t="shared" ref="AC79:AC83" si="152">$E79*AB79</f>
+        <f t="shared" ref="AC79" si="152">$E79*AB79</f>
         <v>0</v>
       </c>
     </row>
@@ -24332,7 +24332,7 @@
         <v>30</v>
       </c>
       <c r="M81" s="41">
-        <f t="shared" ref="M81:M85" si="153">$E81*L81</f>
+        <f t="shared" ref="M81:M83" si="153">$E81*L81</f>
         <v>60</v>
       </c>
       <c r="N81" s="4">
@@ -24347,7 +24347,7 @@
         <v>2.5</v>
       </c>
       <c r="Q81" s="41">
-        <f t="shared" ref="Q81:Q85" si="154">$E81*P81</f>
+        <f t="shared" ref="Q81:Q83" si="154">$E81*P81</f>
         <v>5</v>
       </c>
       <c r="R81" s="4">
@@ -24362,7 +24362,7 @@
         <v>7.5</v>
       </c>
       <c r="U81" s="41">
-        <f t="shared" ref="U81:U85" si="155">$E81*T81</f>
+        <f t="shared" ref="U81:U83" si="155">$E81*T81</f>
         <v>15</v>
       </c>
       <c r="V81" s="4">
@@ -24377,7 +24377,7 @@
         <v>45</v>
       </c>
       <c r="Y81" s="41">
-        <f t="shared" ref="Y81:Y85" si="156">$E81*X81</f>
+        <f t="shared" ref="Y81:Y83" si="156">$E81*X81</f>
         <v>90</v>
       </c>
       <c r="Z81" s="4">
@@ -24392,7 +24392,7 @@
         <v>35</v>
       </c>
       <c r="AC81" s="41">
-        <f t="shared" ref="AC81:AC85" si="157">$E81*AB81</f>
+        <f t="shared" ref="AC81:AC83" si="157">$E81*AB81</f>
         <v>70</v>
       </c>
     </row>
@@ -25516,8 +25516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC93"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView topLeftCell="B1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27816,7 +27816,7 @@
         <v>301</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D25" s="29" t="s">
         <v>383</v>
@@ -30133,8 +30133,8 @@
         <v>1.5</v>
       </c>
       <c r="E48" s="31">
-        <f>1/(0.05*1.5)</f>
-        <v>13.333333333333332</v>
+        <f>1/(0.05*1.5)*0.33</f>
+        <v>4.3999999999999995</v>
       </c>
       <c r="F48" s="4">
         <v>4</v>
@@ -30149,7 +30149,7 @@
       </c>
       <c r="I48" s="12">
         <f t="shared" ref="I48:I53" si="105">$E48*H48</f>
-        <v>4</v>
+        <v>1.32</v>
       </c>
       <c r="J48" s="4">
         <v>1</v>
@@ -30164,7 +30164,7 @@
       </c>
       <c r="M48" s="12">
         <f t="shared" ref="M48:M55" si="107">$E48*L48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="O48" s="5">
         <f>$C48*N48</f>
@@ -30191,7 +30191,7 @@
       </c>
       <c r="U48" s="12">
         <f t="shared" ref="U48:U55" si="111">$E48*T48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="V48" s="4">
         <v>1</v>
@@ -30206,7 +30206,7 @@
       </c>
       <c r="Y48" s="12">
         <f t="shared" ref="Y48:Y55" si="113">$E48*X48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="Z48" s="4">
         <v>0.5</v>
@@ -30221,7 +30221,7 @@
       </c>
       <c r="AC48" s="12">
         <f t="shared" ref="AC48:AC55" si="115">$E48*AB48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30239,8 +30239,8 @@
         <v>1.5</v>
       </c>
       <c r="E49" s="31">
-        <f xml:space="preserve"> 1/(0.05*1.5)</f>
-        <v>13.333333333333332</v>
+        <f>1/(0.05*1.5)*0.33</f>
+        <v>4.3999999999999995</v>
       </c>
       <c r="F49" s="4">
         <v>70</v>
@@ -30255,7 +30255,7 @@
       </c>
       <c r="I49" s="12">
         <f t="shared" si="105"/>
-        <v>70</v>
+        <v>23.099999999999998</v>
       </c>
       <c r="J49" s="4">
         <v>50</v>
@@ -30270,7 +30270,7 @@
       </c>
       <c r="M49" s="12">
         <f t="shared" si="107"/>
-        <v>49.999999999999993</v>
+        <v>16.499999999999996</v>
       </c>
       <c r="O49" s="5">
         <f t="shared" ref="O49:O58" si="117">$C49*N49</f>
@@ -30297,7 +30297,7 @@
       </c>
       <c r="U49" s="12">
         <f t="shared" si="111"/>
-        <v>29.999999999999996</v>
+        <v>9.8999999999999986</v>
       </c>
       <c r="V49" s="4">
         <v>40</v>
@@ -30312,7 +30312,7 @@
       </c>
       <c r="Y49" s="12">
         <f t="shared" si="113"/>
-        <v>40</v>
+        <v>13.2</v>
       </c>
       <c r="Z49" s="4">
         <v>15</v>
@@ -30327,7 +30327,7 @@
       </c>
       <c r="AC49" s="12">
         <f t="shared" si="115"/>
-        <v>14.999999999999998</v>
+        <v>4.9499999999999993</v>
       </c>
     </row>
     <row r="50" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30345,8 +30345,8 @@
         <v>1.5</v>
       </c>
       <c r="E50" s="31">
-        <f xml:space="preserve"> 1/(0.05*1.5)</f>
-        <v>13.333333333333332</v>
+        <f>1/(0.05*1.5)*0.33</f>
+        <v>4.3999999999999995</v>
       </c>
       <c r="F50" s="4">
         <v>2</v>
@@ -30361,7 +30361,7 @@
       </c>
       <c r="I50" s="12">
         <f t="shared" si="105"/>
-        <v>2</v>
+        <v>0.66</v>
       </c>
       <c r="J50" s="4">
         <v>1</v>
@@ -30376,7 +30376,7 @@
       </c>
       <c r="M50" s="12">
         <f t="shared" si="107"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="O50" s="5">
         <f t="shared" si="117"/>
@@ -30403,7 +30403,7 @@
       </c>
       <c r="U50" s="12">
         <f t="shared" si="111"/>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="V50" s="4">
         <v>1</v>
@@ -30418,7 +30418,7 @@
       </c>
       <c r="Y50" s="12">
         <f t="shared" si="113"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="Z50" s="4">
         <v>0.3</v>
@@ -30433,7 +30433,7 @@
       </c>
       <c r="AC50" s="12">
         <f t="shared" si="115"/>
-        <v>0.3</v>
+        <v>9.8999999999999991E-2</v>
       </c>
     </row>
     <row r="51" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30451,8 +30451,8 @@
         <v>1.5</v>
       </c>
       <c r="E51" s="31">
-        <f xml:space="preserve"> 1/(0.05*1.5)</f>
-        <v>13.333333333333332</v>
+        <f>1/(0.05*1.5)*0.33</f>
+        <v>4.3999999999999995</v>
       </c>
       <c r="F51" s="4">
         <v>1.5</v>
@@ -30467,7 +30467,7 @@
       </c>
       <c r="I51" s="12">
         <f t="shared" si="105"/>
-        <v>1.5</v>
+        <v>0.495</v>
       </c>
       <c r="J51" s="4">
         <v>1</v>
@@ -30482,7 +30482,7 @@
       </c>
       <c r="M51" s="12">
         <f t="shared" si="107"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="O51" s="5">
         <f t="shared" si="117"/>
@@ -30509,7 +30509,7 @@
       </c>
       <c r="U51" s="12">
         <f t="shared" si="111"/>
-        <v>0.2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="V51" s="4">
         <v>0.5</v>
@@ -30524,7 +30524,7 @@
       </c>
       <c r="Y51" s="12">
         <f t="shared" si="113"/>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="Z51" s="4">
         <v>0.4</v>
@@ -30539,7 +30539,7 @@
       </c>
       <c r="AC51" s="12">
         <f t="shared" si="115"/>
-        <v>0.4</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30557,8 +30557,8 @@
         <v>1.5</v>
       </c>
       <c r="E52" s="31">
-        <f xml:space="preserve"> 1/(0.05*1.5)</f>
-        <v>13.333333333333332</v>
+        <f>1/(0.05*1.5)*0.33</f>
+        <v>4.3999999999999995</v>
       </c>
       <c r="F52" s="4">
         <v>1</v>
@@ -30573,7 +30573,7 @@
       </c>
       <c r="I52" s="12">
         <f t="shared" si="105"/>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="J52" s="4">
         <v>0.5</v>
@@ -30588,7 +30588,7 @@
       </c>
       <c r="M52" s="12">
         <f t="shared" si="107"/>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="O52" s="5">
         <f t="shared" si="117"/>
@@ -30615,7 +30615,7 @@
       </c>
       <c r="U52" s="12">
         <f t="shared" si="111"/>
-        <v>0.1</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="V52" s="4">
         <v>0.3</v>
@@ -30630,7 +30630,7 @@
       </c>
       <c r="Y52" s="12">
         <f t="shared" si="113"/>
-        <v>0.3</v>
+        <v>9.8999999999999991E-2</v>
       </c>
       <c r="Z52" s="4">
         <v>0.02</v>
@@ -30645,7 +30645,7 @@
       </c>
       <c r="AC52" s="12">
         <f t="shared" si="115"/>
-        <v>1.9999999999999997E-2</v>
+        <v>6.5999999999999991E-3</v>
       </c>
     </row>
     <row r="53" spans="1:29" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -30975,10 +30975,10 @@
         <v>0.5</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E56" s="31" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F56" s="4">
         <v>5</v>
@@ -31074,10 +31074,10 @@
         <v>0.5</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E57" s="31" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="F57" s="4">
         <v>11</v>
@@ -31173,10 +31173,10 @@
         <v>0.5</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E58" s="31" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F58" s="4">
         <v>0</v>
@@ -46088,7 +46088,7 @@
       </c>
       <c r="H48">
         <f>'12_Fire_ModSeverity'!I48</f>
-        <v>4</v>
+        <v>1.32</v>
       </c>
       <c r="I48">
         <f>'13_Fire_HighSeverity'!G48</f>
@@ -46100,7 +46100,7 @@
       </c>
       <c r="K48">
         <f>'13_Fire_HighSeverity'!I48</f>
-        <v>4</v>
+        <v>1.32</v>
       </c>
       <c r="L48">
         <f>'11_Fire_LowSeverity'!J48</f>
@@ -46128,7 +46128,7 @@
       </c>
       <c r="R48">
         <f>'12_Fire_ModSeverity'!M48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="S48">
         <f>'13_Fire_HighSeverity'!K48</f>
@@ -46140,7 +46140,7 @@
       </c>
       <c r="U48">
         <f>'13_Fire_HighSeverity'!M48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="V48">
         <f>'11_Fire_LowSeverity'!N48</f>
@@ -46208,7 +46208,7 @@
       </c>
       <c r="AL48">
         <f>'12_Fire_ModSeverity'!U48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="AM48">
         <f>'13_Fire_HighSeverity'!S48</f>
@@ -46220,7 +46220,7 @@
       </c>
       <c r="AO48">
         <f>'13_Fire_HighSeverity'!U48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="AP48">
         <f>'11_Fire_LowSeverity'!V48</f>
@@ -46248,7 +46248,7 @@
       </c>
       <c r="AV48">
         <f>'12_Fire_ModSeverity'!Y48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AW48">
         <f>'13_Fire_HighSeverity'!W48</f>
@@ -46260,7 +46260,7 @@
       </c>
       <c r="AY48">
         <f>'13_Fire_HighSeverity'!Y48</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AZ48">
         <f>'11_Fire_LowSeverity'!Z48</f>
@@ -46288,7 +46288,7 @@
       </c>
       <c r="BF48">
         <f>'12_Fire_ModSeverity'!AC48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="BG48">
         <f>'13_Fire_HighSeverity'!AA48</f>
@@ -46300,7 +46300,7 @@
       </c>
       <c r="BI48">
         <f>'13_Fire_HighSeverity'!AC48</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
     </row>
     <row r="49" spans="1:61" x14ac:dyDescent="0.25">
@@ -46334,7 +46334,7 @@
       </c>
       <c r="H49">
         <f>'12_Fire_ModSeverity'!I49</f>
-        <v>70</v>
+        <v>23.1</v>
       </c>
       <c r="I49">
         <f>'13_Fire_HighSeverity'!G49</f>
@@ -46346,7 +46346,7 @@
       </c>
       <c r="K49">
         <f>'13_Fire_HighSeverity'!I49</f>
-        <v>70</v>
+        <v>23.099999999999998</v>
       </c>
       <c r="L49">
         <f>'11_Fire_LowSeverity'!J49</f>
@@ -46374,7 +46374,7 @@
       </c>
       <c r="R49">
         <f>'12_Fire_ModSeverity'!M49</f>
-        <v>50</v>
+        <v>16.5</v>
       </c>
       <c r="S49">
         <f>'13_Fire_HighSeverity'!K49</f>
@@ -46386,7 +46386,7 @@
       </c>
       <c r="U49">
         <f>'13_Fire_HighSeverity'!M49</f>
-        <v>49.999999999999993</v>
+        <v>16.499999999999996</v>
       </c>
       <c r="V49">
         <f>'11_Fire_LowSeverity'!N49</f>
@@ -46454,7 +46454,7 @@
       </c>
       <c r="AL49">
         <f>'12_Fire_ModSeverity'!U49</f>
-        <v>30</v>
+        <v>9.9</v>
       </c>
       <c r="AM49">
         <f>'13_Fire_HighSeverity'!S49</f>
@@ -46466,7 +46466,7 @@
       </c>
       <c r="AO49">
         <f>'13_Fire_HighSeverity'!U49</f>
-        <v>29.999999999999996</v>
+        <v>9.8999999999999986</v>
       </c>
       <c r="AP49">
         <f>'11_Fire_LowSeverity'!V49</f>
@@ -46494,7 +46494,7 @@
       </c>
       <c r="AV49">
         <f>'12_Fire_ModSeverity'!Y49</f>
-        <v>40</v>
+        <v>13.200000000000001</v>
       </c>
       <c r="AW49">
         <f>'13_Fire_HighSeverity'!W49</f>
@@ -46506,7 +46506,7 @@
       </c>
       <c r="AY49">
         <f>'13_Fire_HighSeverity'!Y49</f>
-        <v>40</v>
+        <v>13.2</v>
       </c>
       <c r="AZ49">
         <f>'11_Fire_LowSeverity'!Z49</f>
@@ -46534,7 +46534,7 @@
       </c>
       <c r="BF49">
         <f>'12_Fire_ModSeverity'!AC49</f>
-        <v>15</v>
+        <v>4.95</v>
       </c>
       <c r="BG49">
         <f>'13_Fire_HighSeverity'!AA49</f>
@@ -46546,7 +46546,7 @@
       </c>
       <c r="BI49">
         <f>'13_Fire_HighSeverity'!AC49</f>
-        <v>14.999999999999998</v>
+        <v>4.9499999999999993</v>
       </c>
     </row>
     <row r="50" spans="1:61" x14ac:dyDescent="0.25">
@@ -46580,7 +46580,7 @@
       </c>
       <c r="H50">
         <f>'12_Fire_ModSeverity'!I50</f>
-        <v>2</v>
+        <v>0.66</v>
       </c>
       <c r="I50">
         <f>'13_Fire_HighSeverity'!G50</f>
@@ -46592,7 +46592,7 @@
       </c>
       <c r="K50">
         <f>'13_Fire_HighSeverity'!I50</f>
-        <v>2</v>
+        <v>0.66</v>
       </c>
       <c r="L50">
         <f>'11_Fire_LowSeverity'!J50</f>
@@ -46620,7 +46620,7 @@
       </c>
       <c r="R50">
         <f>'12_Fire_ModSeverity'!M50</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="S50">
         <f>'13_Fire_HighSeverity'!K50</f>
@@ -46632,7 +46632,7 @@
       </c>
       <c r="U50">
         <f>'13_Fire_HighSeverity'!M50</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="V50">
         <f>'11_Fire_LowSeverity'!N50</f>
@@ -46700,7 +46700,7 @@
       </c>
       <c r="AL50">
         <f>'12_Fire_ModSeverity'!U50</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="AM50">
         <f>'13_Fire_HighSeverity'!S50</f>
@@ -46712,7 +46712,7 @@
       </c>
       <c r="AO50">
         <f>'13_Fire_HighSeverity'!U50</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="AP50">
         <f>'11_Fire_LowSeverity'!V50</f>
@@ -46740,7 +46740,7 @@
       </c>
       <c r="AV50">
         <f>'12_Fire_ModSeverity'!Y50</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AW50">
         <f>'13_Fire_HighSeverity'!W50</f>
@@ -46752,7 +46752,7 @@
       </c>
       <c r="AY50">
         <f>'13_Fire_HighSeverity'!Y50</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="AZ50">
         <f>'11_Fire_LowSeverity'!Z50</f>
@@ -46780,7 +46780,7 @@
       </c>
       <c r="BF50">
         <f>'12_Fire_ModSeverity'!AC50</f>
-        <v>0.30000000000000004</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="BG50">
         <f>'13_Fire_HighSeverity'!AA50</f>
@@ -46792,7 +46792,7 @@
       </c>
       <c r="BI50">
         <f>'13_Fire_HighSeverity'!AC50</f>
-        <v>0.3</v>
+        <v>9.8999999999999991E-2</v>
       </c>
     </row>
     <row r="51" spans="1:61" x14ac:dyDescent="0.25">
@@ -46826,7 +46826,7 @@
       </c>
       <c r="H51">
         <f>'12_Fire_ModSeverity'!I51</f>
-        <v>1.5</v>
+        <v>0.495</v>
       </c>
       <c r="I51">
         <f>'13_Fire_HighSeverity'!G51</f>
@@ -46838,7 +46838,7 @@
       </c>
       <c r="K51">
         <f>'13_Fire_HighSeverity'!I51</f>
-        <v>1.5</v>
+        <v>0.495</v>
       </c>
       <c r="L51">
         <f>'11_Fire_LowSeverity'!J51</f>
@@ -46866,7 +46866,7 @@
       </c>
       <c r="R51">
         <f>'12_Fire_ModSeverity'!M51</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="S51">
         <f>'13_Fire_HighSeverity'!K51</f>
@@ -46878,7 +46878,7 @@
       </c>
       <c r="U51">
         <f>'13_Fire_HighSeverity'!M51</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="V51">
         <f>'11_Fire_LowSeverity'!N51</f>
@@ -46946,7 +46946,7 @@
       </c>
       <c r="AL51">
         <f>'12_Fire_ModSeverity'!U51</f>
-        <v>0.2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="AM51">
         <f>'13_Fire_HighSeverity'!S51</f>
@@ -46958,7 +46958,7 @@
       </c>
       <c r="AO51">
         <f>'13_Fire_HighSeverity'!U51</f>
-        <v>0.2</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="AP51">
         <f>'11_Fire_LowSeverity'!V51</f>
@@ -46986,7 +46986,7 @@
       </c>
       <c r="AV51">
         <f>'12_Fire_ModSeverity'!Y51</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="AW51">
         <f>'13_Fire_HighSeverity'!W51</f>
@@ -46998,7 +46998,7 @@
       </c>
       <c r="AY51">
         <f>'13_Fire_HighSeverity'!Y51</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="AZ51">
         <f>'11_Fire_LowSeverity'!Z51</f>
@@ -47026,7 +47026,7 @@
       </c>
       <c r="BF51">
         <f>'12_Fire_ModSeverity'!AC51</f>
-        <v>0.4</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="BG51">
         <f>'13_Fire_HighSeverity'!AA51</f>
@@ -47038,7 +47038,7 @@
       </c>
       <c r="BI51">
         <f>'13_Fire_HighSeverity'!AC51</f>
-        <v>0.4</v>
+        <v>0.13200000000000001</v>
       </c>
     </row>
     <row r="52" spans="1:61" x14ac:dyDescent="0.25">
@@ -47072,7 +47072,7 @@
       </c>
       <c r="H52">
         <f>'12_Fire_ModSeverity'!I52</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="I52">
         <f>'13_Fire_HighSeverity'!G52</f>
@@ -47084,7 +47084,7 @@
       </c>
       <c r="K52">
         <f>'13_Fire_HighSeverity'!I52</f>
-        <v>1</v>
+        <v>0.33</v>
       </c>
       <c r="L52">
         <f>'11_Fire_LowSeverity'!J52</f>
@@ -47112,7 +47112,7 @@
       </c>
       <c r="R52">
         <f>'12_Fire_ModSeverity'!M52</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="S52">
         <f>'13_Fire_HighSeverity'!K52</f>
@@ -47124,7 +47124,7 @@
       </c>
       <c r="U52">
         <f>'13_Fire_HighSeverity'!M52</f>
-        <v>0.5</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="V52">
         <f>'11_Fire_LowSeverity'!N52</f>
@@ -47192,7 +47192,7 @@
       </c>
       <c r="AL52">
         <f>'12_Fire_ModSeverity'!U52</f>
-        <v>0.1</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="AM52">
         <f>'13_Fire_HighSeverity'!S52</f>
@@ -47204,7 +47204,7 @@
       </c>
       <c r="AO52">
         <f>'13_Fire_HighSeverity'!U52</f>
-        <v>0.1</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="AP52">
         <f>'11_Fire_LowSeverity'!V52</f>
@@ -47232,7 +47232,7 @@
       </c>
       <c r="AV52">
         <f>'12_Fire_ModSeverity'!Y52</f>
-        <v>0.30000000000000004</v>
+        <v>9.9000000000000005E-2</v>
       </c>
       <c r="AW52">
         <f>'13_Fire_HighSeverity'!W52</f>
@@ -47244,7 +47244,7 @@
       </c>
       <c r="AY52">
         <f>'13_Fire_HighSeverity'!Y52</f>
-        <v>0.3</v>
+        <v>9.8999999999999991E-2</v>
       </c>
       <c r="AZ52">
         <f>'11_Fire_LowSeverity'!Z52</f>
@@ -47272,7 +47272,7 @@
       </c>
       <c r="BF52">
         <f>'12_Fire_ModSeverity'!AC52</f>
-        <v>2.0000000000000004E-2</v>
+        <v>6.6000000000000008E-3</v>
       </c>
       <c r="BG52">
         <f>'13_Fire_HighSeverity'!AA52</f>
@@ -47284,7 +47284,7 @@
       </c>
       <c r="BI52">
         <f>'13_Fire_HighSeverity'!AC52</f>
-        <v>1.9999999999999997E-2</v>
+        <v>6.5999999999999991E-3</v>
       </c>
     </row>
     <row r="53" spans="1:61" x14ac:dyDescent="0.25">

</xml_diff>